<commit_message>
Correção de REDME e correções diversas
</commit_message>
<xml_diff>
--- a/Planilhas/analise_logistica.xlsx
+++ b/Planilhas/analise_logistica.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pedro\Documents\DADOS\Analise IFood GPT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pedro\Documents\DADOS\Analise IFood GPT\ifood_data_analysis\Planilhas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81268A12-B4FD-4C8B-86D1-2A6C27C74D26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFA7D73B-628F-459D-92A9-B8BBEE7D95CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="2655" windowWidth="20730" windowHeight="11310" firstSheet="6" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20610" yWindow="2655" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="clientes" sheetId="1" r:id="rId1"/>
@@ -1370,10 +1370,10 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -15225,8 +15225,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA201"/>
   <sheetViews>
-    <sheetView topLeftCell="S1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AB17" sqref="AB17"/>
+    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection sqref="A1:Y1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15383,7 +15383,7 @@
       </c>
       <c r="L2" s="5">
         <f ca="1">DATEDIF(F2,TODAY(),"D")</f>
-        <v>828</v>
+        <v>836</v>
       </c>
       <c r="M2" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A2),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A2),"")</f>
@@ -15478,7 +15478,7 @@
       </c>
       <c r="L3" s="5">
         <f t="shared" ref="L3:L66" ca="1" si="3">DATEDIF(F3,TODAY(),"D")</f>
-        <v>1639</v>
+        <v>1647</v>
       </c>
       <c r="M3" s="7" t="str">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A3),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A3),"")</f>
@@ -15572,7 +15572,7 @@
       </c>
       <c r="L4" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>1132</v>
+        <v>1140</v>
       </c>
       <c r="M4" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A4),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A4),"")</f>
@@ -15666,7 +15666,7 @@
       </c>
       <c r="L5" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>1223</v>
+        <v>1231</v>
       </c>
       <c r="M5" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A5),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A5),"")</f>
@@ -15757,7 +15757,7 @@
       </c>
       <c r="L6" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>1742</v>
+        <v>1750</v>
       </c>
       <c r="M6" s="7" t="str">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A6),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A6),"")</f>
@@ -15851,7 +15851,7 @@
       </c>
       <c r="L7" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>841</v>
+        <v>849</v>
       </c>
       <c r="M7" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A7),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A7),"")</f>
@@ -15942,7 +15942,7 @@
       </c>
       <c r="L8" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>1366</v>
+        <v>1374</v>
       </c>
       <c r="M8" s="7" t="str">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A8),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A8),"")</f>
@@ -16036,7 +16036,7 @@
       </c>
       <c r="L9" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>1163</v>
+        <v>1171</v>
       </c>
       <c r="M9" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A9),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A9),"")</f>
@@ -16127,7 +16127,7 @@
       </c>
       <c r="L10" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>1192</v>
+        <v>1200</v>
       </c>
       <c r="M10" s="7" t="str">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A10),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A10),"")</f>
@@ -16221,7 +16221,7 @@
       </c>
       <c r="L11" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>1091</v>
+        <v>1099</v>
       </c>
       <c r="M11" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A11),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A11),"")</f>
@@ -16312,7 +16312,7 @@
       </c>
       <c r="L12" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>1742</v>
+        <v>1750</v>
       </c>
       <c r="M12" s="7" t="str">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A12),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A12),"")</f>
@@ -16406,7 +16406,7 @@
       </c>
       <c r="L13" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>1684</v>
+        <v>1692</v>
       </c>
       <c r="M13" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A13),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A13),"")</f>
@@ -16500,7 +16500,7 @@
       </c>
       <c r="L14" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="M14" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A14),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A14),"")</f>
@@ -16591,7 +16591,7 @@
       </c>
       <c r="L15" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>1331</v>
+        <v>1339</v>
       </c>
       <c r="M15" s="7" t="str">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A15),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A15),"")</f>
@@ -16685,7 +16685,7 @@
       </c>
       <c r="L16" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>1631</v>
+        <v>1639</v>
       </c>
       <c r="M16" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A16),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A16),"")</f>
@@ -16776,7 +16776,7 @@
       </c>
       <c r="L17" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>882</v>
+        <v>890</v>
       </c>
       <c r="M17" s="7" t="str">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A17),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A17),"")</f>
@@ -16867,7 +16867,7 @@
       </c>
       <c r="L18" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>1297</v>
+        <v>1305</v>
       </c>
       <c r="M18" s="7" t="str">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A18),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A18),"")</f>
@@ -16961,7 +16961,7 @@
       </c>
       <c r="L19" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>1583</v>
+        <v>1591</v>
       </c>
       <c r="M19" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A19),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A19),"")</f>
@@ -17055,7 +17055,7 @@
       </c>
       <c r="L20" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>1718</v>
+        <v>1726</v>
       </c>
       <c r="M20" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A20),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A20),"")</f>
@@ -17149,7 +17149,7 @@
       </c>
       <c r="L21" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>1503</v>
+        <v>1511</v>
       </c>
       <c r="M21" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A21),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A21),"")</f>
@@ -17243,7 +17243,7 @@
       </c>
       <c r="L22" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>1381</v>
+        <v>1389</v>
       </c>
       <c r="M22" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A22),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A22),"")</f>
@@ -17334,7 +17334,7 @@
       </c>
       <c r="L23" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>1434</v>
+        <v>1442</v>
       </c>
       <c r="M23" s="7" t="str">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A23),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A23),"")</f>
@@ -17425,7 +17425,7 @@
       </c>
       <c r="L24" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>1553</v>
+        <v>1561</v>
       </c>
       <c r="M24" s="7" t="str">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A24),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A24),"")</f>
@@ -17519,7 +17519,7 @@
       </c>
       <c r="L25" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>1304</v>
+        <v>1312</v>
       </c>
       <c r="M25" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A25),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A25),"")</f>
@@ -17610,7 +17610,7 @@
       </c>
       <c r="L26" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>1435</v>
+        <v>1443</v>
       </c>
       <c r="M26" s="7" t="str">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A26),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A26),"")</f>
@@ -17704,7 +17704,7 @@
       </c>
       <c r="L27" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>1424</v>
+        <v>1432</v>
       </c>
       <c r="M27" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A27),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A27),"")</f>
@@ -17795,7 +17795,7 @@
       </c>
       <c r="L28" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>990</v>
+        <v>998</v>
       </c>
       <c r="M28" s="7" t="str">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A28),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A28),"")</f>
@@ -17889,7 +17889,7 @@
       </c>
       <c r="L29" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>869</v>
+        <v>877</v>
       </c>
       <c r="M29" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A29),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A29),"")</f>
@@ -17980,7 +17980,7 @@
       </c>
       <c r="L30" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>1381</v>
+        <v>1389</v>
       </c>
       <c r="M30" s="7" t="str">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A30),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A30),"")</f>
@@ -18071,7 +18071,7 @@
       </c>
       <c r="L31" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>1485</v>
+        <v>1493</v>
       </c>
       <c r="M31" s="7" t="str">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A31),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A31),"")</f>
@@ -18162,7 +18162,7 @@
       </c>
       <c r="L32" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>999</v>
+        <v>1007</v>
       </c>
       <c r="M32" s="7" t="str">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A32),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A32),"")</f>
@@ -18253,7 +18253,7 @@
       </c>
       <c r="L33" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>795</v>
+        <v>803</v>
       </c>
       <c r="M33" s="7" t="str">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A33),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A33),"")</f>
@@ -18347,7 +18347,7 @@
       </c>
       <c r="L34" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>918</v>
+        <v>926</v>
       </c>
       <c r="M34" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A34),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A34),"")</f>
@@ -18438,7 +18438,7 @@
       </c>
       <c r="L35" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>1338</v>
+        <v>1346</v>
       </c>
       <c r="M35" s="7" t="str">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A35),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A35),"")</f>
@@ -18532,7 +18532,7 @@
       </c>
       <c r="L36" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>1511</v>
+        <v>1519</v>
       </c>
       <c r="M36" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A36),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A36),"")</f>
@@ -18623,7 +18623,7 @@
       </c>
       <c r="L37" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>915</v>
+        <v>923</v>
       </c>
       <c r="M37" s="7" t="str">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A37),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A37),"")</f>
@@ -18717,7 +18717,7 @@
       </c>
       <c r="L38" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>1686</v>
+        <v>1694</v>
       </c>
       <c r="M38" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A38),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A38),"")</f>
@@ -18811,7 +18811,7 @@
       </c>
       <c r="L39" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>1288</v>
+        <v>1296</v>
       </c>
       <c r="M39" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A39),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A39),"")</f>
@@ -18905,7 +18905,7 @@
       </c>
       <c r="L40" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>1750</v>
+        <v>1758</v>
       </c>
       <c r="M40" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A40),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A40),"")</f>
@@ -18999,7 +18999,7 @@
       </c>
       <c r="L41" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>1002</v>
+        <v>1010</v>
       </c>
       <c r="M41" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A41),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A41),"")</f>
@@ -19093,7 +19093,7 @@
       </c>
       <c r="L42" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>1217</v>
+        <v>1225</v>
       </c>
       <c r="M42" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A42),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A42),"")</f>
@@ -19184,7 +19184,7 @@
       </c>
       <c r="L43" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>1716</v>
+        <v>1724</v>
       </c>
       <c r="M43" s="7" t="str">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A43),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A43),"")</f>
@@ -19278,7 +19278,7 @@
       </c>
       <c r="L44" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>795</v>
+        <v>803</v>
       </c>
       <c r="M44" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A44),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A44),"")</f>
@@ -19326,11 +19326,11 @@
       </c>
       <c r="X44" t="str">
         <f ca="1">transacao_total!I44</f>
-        <v>Clientes fieis</v>
+        <v>Lealdade potencial</v>
       </c>
       <c r="Y44">
         <f ca="1">transacao_total!J44</f>
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="45" spans="1:25" x14ac:dyDescent="0.25">
@@ -19372,7 +19372,7 @@
       </c>
       <c r="L45" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>1411</v>
+        <v>1419</v>
       </c>
       <c r="M45" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A45),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A45),"")</f>
@@ -19466,7 +19466,7 @@
       </c>
       <c r="L46" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>1540</v>
+        <v>1548</v>
       </c>
       <c r="M46" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A46),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A46),"")</f>
@@ -19557,7 +19557,7 @@
       </c>
       <c r="L47" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>1104</v>
+        <v>1112</v>
       </c>
       <c r="M47" s="7" t="str">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A47),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A47),"")</f>
@@ -19651,7 +19651,7 @@
       </c>
       <c r="L48" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>1699</v>
+        <v>1707</v>
       </c>
       <c r="M48" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A48),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A48),"")</f>
@@ -19742,7 +19742,7 @@
       </c>
       <c r="L49" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>970</v>
+        <v>978</v>
       </c>
       <c r="M49" s="7" t="str">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A49),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A49),"")</f>
@@ -19836,7 +19836,7 @@
       </c>
       <c r="L50" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>789</v>
+        <v>797</v>
       </c>
       <c r="M50" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A50),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A50),"")</f>
@@ -19927,7 +19927,7 @@
       </c>
       <c r="L51" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>1102</v>
+        <v>1110</v>
       </c>
       <c r="M51" s="7" t="str">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A51),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A51),"")</f>
@@ -20021,7 +20021,7 @@
       </c>
       <c r="L52" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>1728</v>
+        <v>1736</v>
       </c>
       <c r="M52" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A52),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A52),"")</f>
@@ -20112,7 +20112,7 @@
       </c>
       <c r="L53" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>997</v>
+        <v>1005</v>
       </c>
       <c r="M53" s="7" t="str">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A53),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A53),"")</f>
@@ -20203,7 +20203,7 @@
       </c>
       <c r="L54" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>1738</v>
+        <v>1746</v>
       </c>
       <c r="M54" s="7" t="str">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A54),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A54),"")</f>
@@ -20294,7 +20294,7 @@
       </c>
       <c r="L55" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>797</v>
+        <v>805</v>
       </c>
       <c r="M55" s="7" t="str">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A55),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A55),"")</f>
@@ -20385,7 +20385,7 @@
       </c>
       <c r="L56" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>1516</v>
+        <v>1524</v>
       </c>
       <c r="M56" s="7" t="str">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A56),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A56),"")</f>
@@ -20476,7 +20476,7 @@
       </c>
       <c r="L57" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>1565</v>
+        <v>1573</v>
       </c>
       <c r="M57" s="7" t="str">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A57),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A57),"")</f>
@@ -20570,7 +20570,7 @@
       </c>
       <c r="L58" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>910</v>
+        <v>918</v>
       </c>
       <c r="M58" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A58),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A58),"")</f>
@@ -20661,7 +20661,7 @@
       </c>
       <c r="L59" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>1749</v>
+        <v>1757</v>
       </c>
       <c r="M59" s="7" t="str">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A59),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A59),"")</f>
@@ -20755,7 +20755,7 @@
       </c>
       <c r="L60" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>1133</v>
+        <v>1141</v>
       </c>
       <c r="M60" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A60),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A60),"")</f>
@@ -20849,7 +20849,7 @@
       </c>
       <c r="L61" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>1613</v>
+        <v>1621</v>
       </c>
       <c r="M61" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A61),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A61),"")</f>
@@ -20943,7 +20943,7 @@
       </c>
       <c r="L62" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>1525</v>
+        <v>1533</v>
       </c>
       <c r="M62" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A62),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A62),"")</f>
@@ -21037,7 +21037,7 @@
       </c>
       <c r="L63" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>1640</v>
+        <v>1648</v>
       </c>
       <c r="M63" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A63),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A63),"")</f>
@@ -21131,7 +21131,7 @@
       </c>
       <c r="L64" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>1285</v>
+        <v>1293</v>
       </c>
       <c r="M64" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A64),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A64),"")</f>
@@ -21222,7 +21222,7 @@
       </c>
       <c r="L65" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>1084</v>
+        <v>1092</v>
       </c>
       <c r="M65" s="7" t="str">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A65),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A65),"")</f>
@@ -21316,7 +21316,7 @@
       </c>
       <c r="L66" s="5">
         <f t="shared" ca="1" si="3"/>
-        <v>1652</v>
+        <v>1660</v>
       </c>
       <c r="M66" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A66),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A66),"")</f>
@@ -21410,7 +21410,7 @@
       </c>
       <c r="L67" s="5">
         <f t="shared" ref="L67:L130" ca="1" si="10">DATEDIF(F67,TODAY(),"D")</f>
-        <v>1192</v>
+        <v>1200</v>
       </c>
       <c r="M67" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A67),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A67),"")</f>
@@ -21458,11 +21458,11 @@
       </c>
       <c r="X67" t="str">
         <f ca="1">transacao_total!I67</f>
-        <v>Clientes que precisam de atenção</v>
+        <v>Em risco</v>
       </c>
       <c r="Y67">
         <f ca="1">transacao_total!J67</f>
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="68" spans="1:25" x14ac:dyDescent="0.25">
@@ -21501,7 +21501,7 @@
       </c>
       <c r="L68" s="5">
         <f t="shared" ca="1" si="10"/>
-        <v>799</v>
+        <v>807</v>
       </c>
       <c r="M68" s="7" t="str">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A68),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A68),"")</f>
@@ -21595,7 +21595,7 @@
       </c>
       <c r="L69" s="5">
         <f t="shared" ca="1" si="10"/>
-        <v>1546</v>
+        <v>1554</v>
       </c>
       <c r="M69" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A69),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A69),"")</f>
@@ -21689,7 +21689,7 @@
       </c>
       <c r="L70" s="5">
         <f t="shared" ca="1" si="10"/>
-        <v>1293</v>
+        <v>1301</v>
       </c>
       <c r="M70" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A70),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A70),"")</f>
@@ -21780,7 +21780,7 @@
       </c>
       <c r="L71" s="5">
         <f t="shared" ca="1" si="10"/>
-        <v>1053</v>
+        <v>1061</v>
       </c>
       <c r="M71" s="7" t="str">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A71),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A71),"")</f>
@@ -21874,7 +21874,7 @@
       </c>
       <c r="L72" s="5">
         <f t="shared" ca="1" si="10"/>
-        <v>1507</v>
+        <v>1515</v>
       </c>
       <c r="M72" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A72),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A72),"")</f>
@@ -21965,7 +21965,7 @@
       </c>
       <c r="L73" s="5">
         <f t="shared" ca="1" si="10"/>
-        <v>984</v>
+        <v>992</v>
       </c>
       <c r="M73" s="7" t="str">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A73),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A73),"")</f>
@@ -22059,7 +22059,7 @@
       </c>
       <c r="L74" s="5">
         <f t="shared" ca="1" si="10"/>
-        <v>1392</v>
+        <v>1400</v>
       </c>
       <c r="M74" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A74),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A74),"")</f>
@@ -22153,7 +22153,7 @@
       </c>
       <c r="L75" s="5">
         <f t="shared" ca="1" si="10"/>
-        <v>1598</v>
+        <v>1606</v>
       </c>
       <c r="M75" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A75),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A75),"")</f>
@@ -22244,7 +22244,7 @@
       </c>
       <c r="L76" s="5">
         <f t="shared" ca="1" si="10"/>
-        <v>1149</v>
+        <v>1157</v>
       </c>
       <c r="M76" s="7" t="str">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A76),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A76),"")</f>
@@ -22338,7 +22338,7 @@
       </c>
       <c r="L77" s="5">
         <f t="shared" ca="1" si="10"/>
-        <v>1148</v>
+        <v>1156</v>
       </c>
       <c r="M77" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A77),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A77),"")</f>
@@ -22432,7 +22432,7 @@
       </c>
       <c r="L78" s="5">
         <f t="shared" ca="1" si="10"/>
-        <v>783</v>
+        <v>791</v>
       </c>
       <c r="M78" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A78),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A78),"")</f>
@@ -22526,7 +22526,7 @@
       </c>
       <c r="L79" s="5">
         <f t="shared" ca="1" si="10"/>
-        <v>1004</v>
+        <v>1012</v>
       </c>
       <c r="M79" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A79),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A79),"")</f>
@@ -22617,7 +22617,7 @@
       </c>
       <c r="L80" s="5">
         <f t="shared" ca="1" si="10"/>
-        <v>1034</v>
+        <v>1042</v>
       </c>
       <c r="M80" s="7" t="str">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A80),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A80),"")</f>
@@ -22708,7 +22708,7 @@
       </c>
       <c r="L81" s="5">
         <f t="shared" ca="1" si="10"/>
-        <v>1652</v>
+        <v>1660</v>
       </c>
       <c r="M81" s="7" t="str">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A81),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A81),"")</f>
@@ -22799,7 +22799,7 @@
       </c>
       <c r="L82" s="5">
         <f t="shared" ca="1" si="10"/>
-        <v>973</v>
+        <v>981</v>
       </c>
       <c r="M82" s="7" t="str">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A82),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A82),"")</f>
@@ -22893,7 +22893,7 @@
       </c>
       <c r="L83" s="5">
         <f t="shared" ca="1" si="10"/>
-        <v>931</v>
+        <v>939</v>
       </c>
       <c r="M83" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A83),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A83),"")</f>
@@ -22987,7 +22987,7 @@
       </c>
       <c r="L84" s="5">
         <f t="shared" ca="1" si="10"/>
-        <v>1602</v>
+        <v>1610</v>
       </c>
       <c r="M84" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A84),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A84),"")</f>
@@ -23081,7 +23081,7 @@
       </c>
       <c r="L85" s="5">
         <f t="shared" ca="1" si="10"/>
-        <v>782</v>
+        <v>790</v>
       </c>
       <c r="M85" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A85),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A85),"")</f>
@@ -23175,7 +23175,7 @@
       </c>
       <c r="L86" s="5">
         <f t="shared" ca="1" si="10"/>
-        <v>1451</v>
+        <v>1459</v>
       </c>
       <c r="M86" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A86),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A86),"")</f>
@@ -23269,7 +23269,7 @@
       </c>
       <c r="L87" s="5">
         <f t="shared" ca="1" si="10"/>
-        <v>1659</v>
+        <v>1667</v>
       </c>
       <c r="M87" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A87),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A87),"")</f>
@@ -23363,7 +23363,7 @@
       </c>
       <c r="L88" s="5">
         <f t="shared" ca="1" si="10"/>
-        <v>1177</v>
+        <v>1185</v>
       </c>
       <c r="M88" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A88),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A88),"")</f>
@@ -23457,7 +23457,7 @@
       </c>
       <c r="L89" s="5">
         <f t="shared" ca="1" si="10"/>
-        <v>1743</v>
+        <v>1751</v>
       </c>
       <c r="M89" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A89),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A89),"")</f>
@@ -23551,7 +23551,7 @@
       </c>
       <c r="L90" s="5">
         <f t="shared" ca="1" si="10"/>
-        <v>818</v>
+        <v>826</v>
       </c>
       <c r="M90" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A90),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A90),"")</f>
@@ -23642,7 +23642,7 @@
       </c>
       <c r="L91" s="5">
         <f t="shared" ca="1" si="10"/>
-        <v>1450</v>
+        <v>1458</v>
       </c>
       <c r="M91" s="7" t="str">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A91),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A91),"")</f>
@@ -23736,7 +23736,7 @@
       </c>
       <c r="L92" s="5">
         <f t="shared" ca="1" si="10"/>
-        <v>1180</v>
+        <v>1188</v>
       </c>
       <c r="M92" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A92),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A92),"")</f>
@@ -23830,7 +23830,7 @@
       </c>
       <c r="L93" s="5">
         <f t="shared" ca="1" si="10"/>
-        <v>1076</v>
+        <v>1084</v>
       </c>
       <c r="M93" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A93),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A93),"")</f>
@@ -23921,7 +23921,7 @@
       </c>
       <c r="L94" s="5">
         <f t="shared" ca="1" si="10"/>
-        <v>840</v>
+        <v>848</v>
       </c>
       <c r="M94" s="7" t="str">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A94),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A94),"")</f>
@@ -24012,7 +24012,7 @@
       </c>
       <c r="L95" s="5">
         <f t="shared" ca="1" si="10"/>
-        <v>788</v>
+        <v>796</v>
       </c>
       <c r="M95" s="7" t="str">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A95),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A95),"")</f>
@@ -24103,7 +24103,7 @@
       </c>
       <c r="L96" s="5">
         <f t="shared" ca="1" si="10"/>
-        <v>1385</v>
+        <v>1393</v>
       </c>
       <c r="M96" s="7" t="str">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A96),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A96),"")</f>
@@ -24197,7 +24197,7 @@
       </c>
       <c r="L97" s="5">
         <f t="shared" ca="1" si="10"/>
-        <v>1363</v>
+        <v>1371</v>
       </c>
       <c r="M97" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A97),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A97),"")</f>
@@ -24291,7 +24291,7 @@
       </c>
       <c r="L98" s="5">
         <f t="shared" ca="1" si="10"/>
-        <v>805</v>
+        <v>813</v>
       </c>
       <c r="M98" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A98),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A98),"")</f>
@@ -24385,7 +24385,7 @@
       </c>
       <c r="L99" s="5">
         <f t="shared" ca="1" si="10"/>
-        <v>1037</v>
+        <v>1045</v>
       </c>
       <c r="M99" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A99),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A99),"")</f>
@@ -24479,7 +24479,7 @@
       </c>
       <c r="L100" s="5">
         <f t="shared" ca="1" si="10"/>
-        <v>1566</v>
+        <v>1574</v>
       </c>
       <c r="M100" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A100),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A100),"")</f>
@@ -24570,7 +24570,7 @@
       </c>
       <c r="L101" s="5">
         <f t="shared" ca="1" si="10"/>
-        <v>1692</v>
+        <v>1700</v>
       </c>
       <c r="M101" s="7" t="str">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A101),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A101),"")</f>
@@ -24661,7 +24661,7 @@
       </c>
       <c r="L102" s="5">
         <f t="shared" ca="1" si="10"/>
-        <v>1163</v>
+        <v>1171</v>
       </c>
       <c r="M102" s="7" t="str">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A102),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A102),"")</f>
@@ -24755,7 +24755,7 @@
       </c>
       <c r="L103" s="5">
         <f t="shared" ca="1" si="10"/>
-        <v>1062</v>
+        <v>1070</v>
       </c>
       <c r="M103" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A103),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A103),"")</f>
@@ -24846,7 +24846,7 @@
       </c>
       <c r="L104" s="5">
         <f t="shared" ca="1" si="10"/>
-        <v>919</v>
+        <v>927</v>
       </c>
       <c r="M104" s="7" t="str">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A104),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A104),"")</f>
@@ -24937,7 +24937,7 @@
       </c>
       <c r="L105" s="5">
         <f t="shared" ca="1" si="10"/>
-        <v>1127</v>
+        <v>1135</v>
       </c>
       <c r="M105" s="7" t="str">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A105),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A105),"")</f>
@@ -25031,7 +25031,7 @@
       </c>
       <c r="L106" s="5">
         <f t="shared" ca="1" si="10"/>
-        <v>1521</v>
+        <v>1529</v>
       </c>
       <c r="M106" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A106),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A106),"")</f>
@@ -25125,7 +25125,7 @@
       </c>
       <c r="L107" s="5">
         <f t="shared" ca="1" si="10"/>
-        <v>1665</v>
+        <v>1673</v>
       </c>
       <c r="M107" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A107),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A107),"")</f>
@@ -25219,7 +25219,7 @@
       </c>
       <c r="L108" s="5">
         <f t="shared" ca="1" si="10"/>
-        <v>1056</v>
+        <v>1064</v>
       </c>
       <c r="M108" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A108),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A108),"")</f>
@@ -25310,7 +25310,7 @@
       </c>
       <c r="L109" s="5">
         <f t="shared" ca="1" si="10"/>
-        <v>978</v>
+        <v>986</v>
       </c>
       <c r="M109" s="7" t="str">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A109),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A109),"")</f>
@@ -25404,7 +25404,7 @@
       </c>
       <c r="L110" s="5">
         <f t="shared" ca="1" si="10"/>
-        <v>1461</v>
+        <v>1469</v>
       </c>
       <c r="M110" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A110),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A110),"")</f>
@@ -25495,7 +25495,7 @@
       </c>
       <c r="L111" s="5">
         <f t="shared" ca="1" si="10"/>
-        <v>899</v>
+        <v>907</v>
       </c>
       <c r="M111" s="7" t="str">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A111),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A111),"")</f>
@@ -25589,7 +25589,7 @@
       </c>
       <c r="L112" s="5">
         <f t="shared" ca="1" si="10"/>
-        <v>1069</v>
+        <v>1077</v>
       </c>
       <c r="M112" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A112),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A112),"")</f>
@@ -25683,7 +25683,7 @@
       </c>
       <c r="L113" s="5">
         <f t="shared" ca="1" si="10"/>
-        <v>1155</v>
+        <v>1163</v>
       </c>
       <c r="M113" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A113),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A113),"")</f>
@@ -25777,7 +25777,7 @@
       </c>
       <c r="L114" s="5">
         <f t="shared" ca="1" si="10"/>
-        <v>945</v>
+        <v>953</v>
       </c>
       <c r="M114" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A114),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A114),"")</f>
@@ -25871,7 +25871,7 @@
       </c>
       <c r="L115" s="5">
         <f t="shared" ca="1" si="10"/>
-        <v>1646</v>
+        <v>1654</v>
       </c>
       <c r="M115" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A115),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A115),"")</f>
@@ -25965,7 +25965,7 @@
       </c>
       <c r="L116" s="5">
         <f t="shared" ca="1" si="10"/>
-        <v>954</v>
+        <v>962</v>
       </c>
       <c r="M116" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A116),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A116),"")</f>
@@ -26056,7 +26056,7 @@
       </c>
       <c r="L117" s="5">
         <f t="shared" ca="1" si="10"/>
-        <v>1190</v>
+        <v>1198</v>
       </c>
       <c r="M117" s="7" t="str">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A117),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A117),"")</f>
@@ -26150,7 +26150,7 @@
       </c>
       <c r="L118" s="5">
         <f t="shared" ca="1" si="10"/>
-        <v>968</v>
+        <v>976</v>
       </c>
       <c r="M118" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A118),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A118),"")</f>
@@ -26244,7 +26244,7 @@
       </c>
       <c r="L119" s="5">
         <f t="shared" ca="1" si="10"/>
-        <v>1727</v>
+        <v>1735</v>
       </c>
       <c r="M119" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A119),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A119),"")</f>
@@ -26338,7 +26338,7 @@
       </c>
       <c r="L120" s="5">
         <f t="shared" ca="1" si="10"/>
-        <v>1414</v>
+        <v>1422</v>
       </c>
       <c r="M120" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A120),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A120),"")</f>
@@ -26432,7 +26432,7 @@
       </c>
       <c r="L121" s="5">
         <f t="shared" ca="1" si="10"/>
-        <v>1224</v>
+        <v>1232</v>
       </c>
       <c r="M121" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A121),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A121),"")</f>
@@ -26526,7 +26526,7 @@
       </c>
       <c r="L122" s="5">
         <f t="shared" ca="1" si="10"/>
-        <v>1331</v>
+        <v>1339</v>
       </c>
       <c r="M122" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A122),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A122),"")</f>
@@ -26620,7 +26620,7 @@
       </c>
       <c r="L123" s="5">
         <f t="shared" ca="1" si="10"/>
-        <v>1092</v>
+        <v>1100</v>
       </c>
       <c r="M123" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A123),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A123),"")</f>
@@ -26711,7 +26711,7 @@
       </c>
       <c r="L124" s="5">
         <f t="shared" ca="1" si="10"/>
-        <v>1390</v>
+        <v>1398</v>
       </c>
       <c r="M124" s="7" t="str">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A124),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A124),"")</f>
@@ -26805,7 +26805,7 @@
       </c>
       <c r="L125" s="5">
         <f t="shared" ca="1" si="10"/>
-        <v>1699</v>
+        <v>1707</v>
       </c>
       <c r="M125" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A125),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A125),"")</f>
@@ -26899,7 +26899,7 @@
       </c>
       <c r="L126" s="5">
         <f t="shared" ca="1" si="10"/>
-        <v>1251</v>
+        <v>1259</v>
       </c>
       <c r="M126" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A126),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A126),"")</f>
@@ -26993,7 +26993,7 @@
       </c>
       <c r="L127" s="5">
         <f t="shared" ca="1" si="10"/>
-        <v>1106</v>
+        <v>1114</v>
       </c>
       <c r="M127" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A127),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A127),"")</f>
@@ -27087,7 +27087,7 @@
       </c>
       <c r="L128" s="5">
         <f t="shared" ca="1" si="10"/>
-        <v>1420</v>
+        <v>1428</v>
       </c>
       <c r="M128" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A128),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A128),"")</f>
@@ -27181,7 +27181,7 @@
       </c>
       <c r="L129" s="5">
         <f t="shared" ca="1" si="10"/>
-        <v>1757</v>
+        <v>1765</v>
       </c>
       <c r="M129" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A129),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A129),"")</f>
@@ -27275,7 +27275,7 @@
       </c>
       <c r="L130" s="5">
         <f t="shared" ca="1" si="10"/>
-        <v>900</v>
+        <v>908</v>
       </c>
       <c r="M130" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A130),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A130),"")</f>
@@ -27369,7 +27369,7 @@
       </c>
       <c r="L131" s="5">
         <f t="shared" ref="L131:L194" ca="1" si="16">DATEDIF(F131,TODAY(),"D")</f>
-        <v>1339</v>
+        <v>1347</v>
       </c>
       <c r="M131" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A131),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A131),"")</f>
@@ -27463,7 +27463,7 @@
       </c>
       <c r="L132" s="5">
         <f t="shared" ca="1" si="16"/>
-        <v>927</v>
+        <v>935</v>
       </c>
       <c r="M132" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A132),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A132),"")</f>
@@ -27554,7 +27554,7 @@
       </c>
       <c r="L133" s="5">
         <f t="shared" ca="1" si="16"/>
-        <v>1268</v>
+        <v>1276</v>
       </c>
       <c r="M133" s="7" t="str">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A133),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A133),"")</f>
@@ -27645,7 +27645,7 @@
       </c>
       <c r="L134" s="5">
         <f t="shared" ca="1" si="16"/>
-        <v>1661</v>
+        <v>1669</v>
       </c>
       <c r="M134" s="7" t="str">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A134),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A134),"")</f>
@@ -27736,7 +27736,7 @@
       </c>
       <c r="L135" s="5">
         <f t="shared" ca="1" si="16"/>
-        <v>1326</v>
+        <v>1334</v>
       </c>
       <c r="M135" s="7" t="str">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A135),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A135),"")</f>
@@ -27830,7 +27830,7 @@
       </c>
       <c r="L136" s="5">
         <f t="shared" ca="1" si="16"/>
-        <v>786</v>
+        <v>794</v>
       </c>
       <c r="M136" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A136),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A136),"")</f>
@@ -27924,7 +27924,7 @@
       </c>
       <c r="L137" s="5">
         <f t="shared" ca="1" si="16"/>
-        <v>1399</v>
+        <v>1407</v>
       </c>
       <c r="M137" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A137),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A137),"")</f>
@@ -28018,7 +28018,7 @@
       </c>
       <c r="L138" s="5">
         <f t="shared" ca="1" si="16"/>
-        <v>1119</v>
+        <v>1127</v>
       </c>
       <c r="M138" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A138),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A138),"")</f>
@@ -28112,7 +28112,7 @@
       </c>
       <c r="L139" s="5">
         <f t="shared" ca="1" si="16"/>
-        <v>857</v>
+        <v>865</v>
       </c>
       <c r="M139" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A139),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A139),"")</f>
@@ -28206,7 +28206,7 @@
       </c>
       <c r="L140" s="5">
         <f t="shared" ca="1" si="16"/>
-        <v>921</v>
+        <v>929</v>
       </c>
       <c r="M140" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A140),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A140),"")</f>
@@ -28300,7 +28300,7 @@
       </c>
       <c r="L141" s="5">
         <f t="shared" ca="1" si="16"/>
-        <v>1299</v>
+        <v>1307</v>
       </c>
       <c r="M141" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A141),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A141),"")</f>
@@ -28391,7 +28391,7 @@
       </c>
       <c r="L142" s="5">
         <f t="shared" ca="1" si="16"/>
-        <v>1045</v>
+        <v>1053</v>
       </c>
       <c r="M142" s="7" t="str">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A142),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A142),"")</f>
@@ -28485,7 +28485,7 @@
       </c>
       <c r="L143" s="5">
         <f t="shared" ca="1" si="16"/>
-        <v>1613</v>
+        <v>1621</v>
       </c>
       <c r="M143" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A143),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A143),"")</f>
@@ -28576,7 +28576,7 @@
       </c>
       <c r="L144" s="5">
         <f t="shared" ca="1" si="16"/>
-        <v>1324</v>
+        <v>1332</v>
       </c>
       <c r="M144" s="7" t="str">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A144),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A144),"")</f>
@@ -28667,7 +28667,7 @@
       </c>
       <c r="L145" s="5">
         <f t="shared" ca="1" si="16"/>
-        <v>1589</v>
+        <v>1597</v>
       </c>
       <c r="M145" s="7" t="str">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A145),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A145),"")</f>
@@ -28761,7 +28761,7 @@
       </c>
       <c r="L146" s="5">
         <f t="shared" ca="1" si="16"/>
-        <v>1018</v>
+        <v>1026</v>
       </c>
       <c r="M146" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A146),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A146),"")</f>
@@ -28852,7 +28852,7 @@
       </c>
       <c r="L147" s="5">
         <f t="shared" ca="1" si="16"/>
-        <v>1235</v>
+        <v>1243</v>
       </c>
       <c r="M147" s="7" t="str">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A147),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A147),"")</f>
@@ -28946,7 +28946,7 @@
       </c>
       <c r="L148" s="5">
         <f t="shared" ca="1" si="16"/>
-        <v>781</v>
+        <v>789</v>
       </c>
       <c r="M148" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A148),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A148),"")</f>
@@ -29040,7 +29040,7 @@
       </c>
       <c r="L149" s="5">
         <f t="shared" ca="1" si="16"/>
-        <v>1103</v>
+        <v>1111</v>
       </c>
       <c r="M149" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A149),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A149),"")</f>
@@ -29134,7 +29134,7 @@
       </c>
       <c r="L150" s="5">
         <f t="shared" ca="1" si="16"/>
-        <v>1493</v>
+        <v>1501</v>
       </c>
       <c r="M150" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A150),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A150),"")</f>
@@ -29228,7 +29228,7 @@
       </c>
       <c r="L151" s="5">
         <f t="shared" ca="1" si="16"/>
-        <v>1139</v>
+        <v>1147</v>
       </c>
       <c r="M151" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A151),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A151),"")</f>
@@ -29322,7 +29322,7 @@
       </c>
       <c r="L152" s="5">
         <f t="shared" ca="1" si="16"/>
-        <v>942</v>
+        <v>950</v>
       </c>
       <c r="M152" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A152),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A152),"")</f>
@@ -29416,7 +29416,7 @@
       </c>
       <c r="L153" s="5">
         <f t="shared" ca="1" si="16"/>
-        <v>828</v>
+        <v>836</v>
       </c>
       <c r="M153" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A153),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A153),"")</f>
@@ -29507,7 +29507,7 @@
       </c>
       <c r="L154" s="5">
         <f t="shared" ca="1" si="16"/>
-        <v>1218</v>
+        <v>1226</v>
       </c>
       <c r="M154" s="7" t="str">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A154),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A154),"")</f>
@@ -29601,7 +29601,7 @@
       </c>
       <c r="L155" s="5">
         <f t="shared" ca="1" si="16"/>
-        <v>976</v>
+        <v>984</v>
       </c>
       <c r="M155" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A155),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A155),"")</f>
@@ -29692,7 +29692,7 @@
       </c>
       <c r="L156" s="5">
         <f t="shared" ca="1" si="16"/>
-        <v>1274</v>
+        <v>1282</v>
       </c>
       <c r="M156" s="7" t="str">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A156),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A156),"")</f>
@@ -29786,7 +29786,7 @@
       </c>
       <c r="L157" s="5">
         <f t="shared" ca="1" si="16"/>
-        <v>1293</v>
+        <v>1301</v>
       </c>
       <c r="M157" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A157),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A157),"")</f>
@@ -29880,7 +29880,7 @@
       </c>
       <c r="L158" s="5">
         <f t="shared" ca="1" si="16"/>
-        <v>1323</v>
+        <v>1331</v>
       </c>
       <c r="M158" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A158),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A158),"")</f>
@@ -29971,7 +29971,7 @@
       </c>
       <c r="L159" s="5">
         <f t="shared" ca="1" si="16"/>
-        <v>924</v>
+        <v>932</v>
       </c>
       <c r="M159" s="7" t="str">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A159),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A159),"")</f>
@@ -30065,7 +30065,7 @@
       </c>
       <c r="L160" s="5">
         <f t="shared" ca="1" si="16"/>
-        <v>1021</v>
+        <v>1029</v>
       </c>
       <c r="M160" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A160),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A160),"")</f>
@@ -30159,7 +30159,7 @@
       </c>
       <c r="L161" s="5">
         <f t="shared" ca="1" si="16"/>
-        <v>1163</v>
+        <v>1171</v>
       </c>
       <c r="M161" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A161),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A161),"")</f>
@@ -30253,7 +30253,7 @@
       </c>
       <c r="L162" s="5">
         <f t="shared" ca="1" si="16"/>
-        <v>1495</v>
+        <v>1503</v>
       </c>
       <c r="M162" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A162),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A162),"")</f>
@@ -30347,7 +30347,7 @@
       </c>
       <c r="L163" s="5">
         <f t="shared" ca="1" si="16"/>
-        <v>1439</v>
+        <v>1447</v>
       </c>
       <c r="M163" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A163),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A163),"")</f>
@@ -30441,7 +30441,7 @@
       </c>
       <c r="L164" s="5">
         <f t="shared" ca="1" si="16"/>
-        <v>897</v>
+        <v>905</v>
       </c>
       <c r="M164" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A164),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A164),"")</f>
@@ -30489,11 +30489,11 @@
       </c>
       <c r="X164" t="str">
         <f ca="1">transacao_total!I164</f>
-        <v>Clientes fieis</v>
+        <v>Clientes que precisam de atenção</v>
       </c>
       <c r="Y164">
         <f ca="1">transacao_total!J164</f>
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="165" spans="1:25" x14ac:dyDescent="0.25">
@@ -30535,7 +30535,7 @@
       </c>
       <c r="L165" s="5">
         <f t="shared" ca="1" si="16"/>
-        <v>1518</v>
+        <v>1526</v>
       </c>
       <c r="M165" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A165),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A165),"")</f>
@@ -30626,7 +30626,7 @@
       </c>
       <c r="L166" s="5">
         <f t="shared" ca="1" si="16"/>
-        <v>919</v>
+        <v>927</v>
       </c>
       <c r="M166" s="7" t="str">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A166),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A166),"")</f>
@@ -30717,7 +30717,7 @@
       </c>
       <c r="L167" s="5">
         <f t="shared" ca="1" si="16"/>
-        <v>812</v>
+        <v>820</v>
       </c>
       <c r="M167" s="7" t="str">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A167),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A167),"")</f>
@@ -30811,7 +30811,7 @@
       </c>
       <c r="L168" s="5">
         <f t="shared" ca="1" si="16"/>
-        <v>1681</v>
+        <v>1689</v>
       </c>
       <c r="M168" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A168),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A168),"")</f>
@@ -30905,7 +30905,7 @@
       </c>
       <c r="L169" s="5">
         <f t="shared" ca="1" si="16"/>
-        <v>1484</v>
+        <v>1492</v>
       </c>
       <c r="M169" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A169),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A169),"")</f>
@@ -30999,7 +30999,7 @@
       </c>
       <c r="L170" s="5">
         <f t="shared" ca="1" si="16"/>
-        <v>867</v>
+        <v>875</v>
       </c>
       <c r="M170" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A170),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A170),"")</f>
@@ -31093,7 +31093,7 @@
       </c>
       <c r="L171" s="5">
         <f t="shared" ca="1" si="16"/>
-        <v>1308</v>
+        <v>1316</v>
       </c>
       <c r="M171" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A171),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A171),"")</f>
@@ -31187,7 +31187,7 @@
       </c>
       <c r="L172" s="5">
         <f t="shared" ca="1" si="16"/>
-        <v>1520</v>
+        <v>1528</v>
       </c>
       <c r="M172" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A172),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A172),"")</f>
@@ -31278,7 +31278,7 @@
       </c>
       <c r="L173" s="5">
         <f t="shared" ca="1" si="16"/>
-        <v>1001</v>
+        <v>1009</v>
       </c>
       <c r="M173" s="7" t="str">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A173),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A173),"")</f>
@@ -31372,7 +31372,7 @@
       </c>
       <c r="L174" s="5">
         <f t="shared" ca="1" si="16"/>
-        <v>1294</v>
+        <v>1302</v>
       </c>
       <c r="M174" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A174),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A174),"")</f>
@@ -31466,7 +31466,7 @@
       </c>
       <c r="L175" s="5">
         <f t="shared" ca="1" si="16"/>
-        <v>1186</v>
+        <v>1194</v>
       </c>
       <c r="M175" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A175),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A175),"")</f>
@@ -31560,7 +31560,7 @@
       </c>
       <c r="L176" s="5">
         <f t="shared" ca="1" si="16"/>
-        <v>1145</v>
+        <v>1153</v>
       </c>
       <c r="M176" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A176),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A176),"")</f>
@@ -31654,7 +31654,7 @@
       </c>
       <c r="L177" s="5">
         <f t="shared" ca="1" si="16"/>
-        <v>1085</v>
+        <v>1093</v>
       </c>
       <c r="M177" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A177),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A177),"")</f>
@@ -31748,7 +31748,7 @@
       </c>
       <c r="L178" s="5">
         <f t="shared" ca="1" si="16"/>
-        <v>1381</v>
+        <v>1389</v>
       </c>
       <c r="M178" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A178),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A178),"")</f>
@@ -31842,7 +31842,7 @@
       </c>
       <c r="L179" s="5">
         <f t="shared" ca="1" si="16"/>
-        <v>1425</v>
+        <v>1433</v>
       </c>
       <c r="M179" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A179),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A179),"")</f>
@@ -31936,7 +31936,7 @@
       </c>
       <c r="L180" s="5">
         <f t="shared" ca="1" si="16"/>
-        <v>1740</v>
+        <v>1748</v>
       </c>
       <c r="M180" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A180),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A180),"")</f>
@@ -32030,7 +32030,7 @@
       </c>
       <c r="L181" s="5">
         <f t="shared" ca="1" si="16"/>
-        <v>1263</v>
+        <v>1271</v>
       </c>
       <c r="M181" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A181),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A181),"")</f>
@@ -32124,7 +32124,7 @@
       </c>
       <c r="L182" s="5">
         <f t="shared" ca="1" si="16"/>
-        <v>898</v>
+        <v>906</v>
       </c>
       <c r="M182" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A182),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A182),"")</f>
@@ -32172,11 +32172,11 @@
       </c>
       <c r="X182" t="str">
         <f ca="1">transacao_total!I182</f>
-        <v>Clientes fieis</v>
+        <v>Clientes que precisam de atenção</v>
       </c>
       <c r="Y182">
         <f ca="1">transacao_total!J182</f>
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="183" spans="1:25" x14ac:dyDescent="0.25">
@@ -32215,7 +32215,7 @@
       </c>
       <c r="L183" s="5">
         <f t="shared" ca="1" si="16"/>
-        <v>1437</v>
+        <v>1445</v>
       </c>
       <c r="M183" s="7" t="str">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A183),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A183),"")</f>
@@ -32306,7 +32306,7 @@
       </c>
       <c r="L184" s="5">
         <f t="shared" ca="1" si="16"/>
-        <v>1583</v>
+        <v>1591</v>
       </c>
       <c r="M184" s="7" t="str">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A184),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A184),"")</f>
@@ -32400,7 +32400,7 @@
       </c>
       <c r="L185" s="5">
         <f t="shared" ca="1" si="16"/>
-        <v>1270</v>
+        <v>1278</v>
       </c>
       <c r="M185" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A185),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A185),"")</f>
@@ -32494,7 +32494,7 @@
       </c>
       <c r="L186" s="5">
         <f t="shared" ca="1" si="16"/>
-        <v>1552</v>
+        <v>1560</v>
       </c>
       <c r="M186" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A186),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A186),"")</f>
@@ -32588,7 +32588,7 @@
       </c>
       <c r="L187" s="5">
         <f t="shared" ca="1" si="16"/>
-        <v>1406</v>
+        <v>1414</v>
       </c>
       <c r="M187" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A187),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A187),"")</f>
@@ -32679,7 +32679,7 @@
       </c>
       <c r="L188" s="5">
         <f t="shared" ca="1" si="16"/>
-        <v>953</v>
+        <v>961</v>
       </c>
       <c r="M188" s="7" t="str">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A188),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A188),"")</f>
@@ -32770,7 +32770,7 @@
       </c>
       <c r="L189" s="5">
         <f t="shared" ca="1" si="16"/>
-        <v>1505</v>
+        <v>1513</v>
       </c>
       <c r="M189" s="7" t="str">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A189),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A189),"")</f>
@@ -32861,7 +32861,7 @@
       </c>
       <c r="L190" s="5">
         <f t="shared" ca="1" si="16"/>
-        <v>1421</v>
+        <v>1429</v>
       </c>
       <c r="M190" s="7" t="str">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A190),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A190),"")</f>
@@ -32952,7 +32952,7 @@
       </c>
       <c r="L191" s="5">
         <f t="shared" ca="1" si="16"/>
-        <v>1483</v>
+        <v>1491</v>
       </c>
       <c r="M191" s="7" t="str">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A191),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A191),"")</f>
@@ -33046,7 +33046,7 @@
       </c>
       <c r="L192" s="5">
         <f t="shared" ca="1" si="16"/>
-        <v>868</v>
+        <v>876</v>
       </c>
       <c r="M192" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A192),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A192),"")</f>
@@ -33140,7 +33140,7 @@
       </c>
       <c r="L193" s="5">
         <f t="shared" ca="1" si="16"/>
-        <v>1159</v>
+        <v>1167</v>
       </c>
       <c r="M193" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A193),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A193),"")</f>
@@ -33231,7 +33231,7 @@
       </c>
       <c r="L194" s="5">
         <f t="shared" ca="1" si="16"/>
-        <v>1051</v>
+        <v>1059</v>
       </c>
       <c r="M194" s="7" t="str">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A194),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A194),"")</f>
@@ -33325,7 +33325,7 @@
       </c>
       <c r="L195" s="5">
         <f t="shared" ref="L195:L201" ca="1" si="22">DATEDIF(F195,TODAY(),"D")</f>
-        <v>868</v>
+        <v>876</v>
       </c>
       <c r="M195" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A195),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A195),"")</f>
@@ -33419,7 +33419,7 @@
       </c>
       <c r="L196" s="5">
         <f t="shared" ca="1" si="22"/>
-        <v>1487</v>
+        <v>1495</v>
       </c>
       <c r="M196" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A196),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A196),"")</f>
@@ -33513,7 +33513,7 @@
       </c>
       <c r="L197" s="5">
         <f t="shared" ca="1" si="22"/>
-        <v>1200</v>
+        <v>1208</v>
       </c>
       <c r="M197" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A197),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A197),"")</f>
@@ -33607,7 +33607,7 @@
       </c>
       <c r="L198" s="5">
         <f t="shared" ca="1" si="22"/>
-        <v>1759</v>
+        <v>1767</v>
       </c>
       <c r="M198" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A198),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A198),"")</f>
@@ -33701,7 +33701,7 @@
       </c>
       <c r="L199" s="5">
         <f t="shared" ca="1" si="22"/>
-        <v>1240</v>
+        <v>1248</v>
       </c>
       <c r="M199" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A199),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A199),"")</f>
@@ -33795,7 +33795,7 @@
       </c>
       <c r="L200" s="5">
         <f t="shared" ca="1" si="22"/>
-        <v>799</v>
+        <v>807</v>
       </c>
       <c r="M200" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A200),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A200),"")</f>
@@ -33889,7 +33889,7 @@
       </c>
       <c r="L201" s="5">
         <f t="shared" ca="1" si="22"/>
-        <v>1574</v>
+        <v>1582</v>
       </c>
       <c r="M201" s="7">
         <f>IF(_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A201),_xlfn.MAXIFS(transacoes!$D$1:$D$201,transacoes!$B$1:$B$201,clientes!A201),"")</f>
@@ -34111,7 +34111,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6025D64-63D2-4ED2-9358-AD33AD78A006}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -34181,7 +34181,7 @@
       <c r="A11" t="s">
         <v>215</v>
       </c>
-      <c r="B11" s="34">
+      <c r="B11" s="33">
         <v>1.03</v>
       </c>
     </row>
@@ -34189,7 +34189,7 @@
       <c r="A12" t="s">
         <v>214</v>
       </c>
-      <c r="B12" s="34">
+      <c r="B12" s="33">
         <v>0.95</v>
       </c>
     </row>
@@ -36014,11 +36014,11 @@
       </c>
       <c r="I44" t="str">
         <f ca="1">'Segmetação demográfica'!H45</f>
-        <v>Clientes fieis</v>
+        <v>Lealdade potencial</v>
       </c>
       <c r="J44">
         <f ca="1">IFERROR(VLOOKUP(I44,'Clientes alto valor'!$H$2:$K$13,4,FALSE),0)</f>
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
@@ -36957,11 +36957,11 @@
       </c>
       <c r="I67" t="str">
         <f ca="1">'Segmetação demográfica'!H68</f>
-        <v>Clientes que precisam de atenção</v>
+        <v>Em risco</v>
       </c>
       <c r="J67">
         <f ca="1">IFERROR(VLOOKUP(I67,'Clientes alto valor'!$H$2:$K$13,4,FALSE),0)</f>
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
@@ -40934,11 +40934,11 @@
       </c>
       <c r="I164" t="str">
         <f ca="1">'Segmetação demográfica'!H165</f>
-        <v>Clientes fieis</v>
+        <v>Clientes que precisam de atenção</v>
       </c>
       <c r="J164">
         <f ca="1">IFERROR(VLOOKUP(I164,'Clientes alto valor'!$H$2:$K$13,4,FALSE),0)</f>
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="165" spans="1:10" x14ac:dyDescent="0.25">
@@ -41672,11 +41672,11 @@
       </c>
       <c r="I182" t="str">
         <f ca="1">'Segmetação demográfica'!H183</f>
-        <v>Clientes fieis</v>
+        <v>Clientes que precisam de atenção</v>
       </c>
       <c r="J182">
         <f ca="1">IFERROR(VLOOKUP(I182,'Clientes alto valor'!$H$2:$K$13,4,FALSE),0)</f>
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="183" spans="1:10" x14ac:dyDescent="0.25">
@@ -42588,10 +42588,10 @@
       <c r="F5" t="s">
         <v>224</v>
       </c>
-      <c r="I5" s="33" t="s">
+      <c r="I5" s="34" t="s">
         <v>289</v>
       </c>
-      <c r="J5" s="33"/>
+      <c r="J5" s="34"/>
       <c r="K5" s="22"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -42977,17 +42977,17 @@
       <c r="F21" t="s">
         <v>224</v>
       </c>
-      <c r="I21" s="33" t="s">
+      <c r="I21" s="34" t="s">
         <v>292</v>
       </c>
-      <c r="J21" s="33"/>
-      <c r="K21" s="33"/>
-      <c r="L21" s="33"/>
+      <c r="J21" s="34"/>
+      <c r="K21" s="34"/>
+      <c r="L21" s="34"/>
       <c r="M21" s="22"/>
-      <c r="Q21" s="33" t="s">
+      <c r="Q21" s="34" t="s">
         <v>301</v>
       </c>
-      <c r="R21" s="33"/>
+      <c r="R21" s="34"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22">
@@ -43067,7 +43067,7 @@
       </c>
       <c r="K23" s="25">
         <f ca="1">VLOOKUP(I23,clientes!$A:$P,12,FALSE)</f>
-        <v>968</v>
+        <v>976</v>
       </c>
       <c r="L23">
         <f t="shared" ref="L23:L54" si="2">COUNTIF(B:B,I23)</f>
@@ -43123,7 +43123,7 @@
       </c>
       <c r="K24" s="25">
         <f ca="1">VLOOKUP(I24,clientes!$A:$P,12,FALSE)</f>
-        <v>1037</v>
+        <v>1045</v>
       </c>
       <c r="L24">
         <f t="shared" si="2"/>
@@ -43179,7 +43179,7 @@
       </c>
       <c r="K25" s="25">
         <f ca="1">VLOOKUP(I25,clientes!$A:$P,12,FALSE)</f>
-        <v>1424</v>
+        <v>1432</v>
       </c>
       <c r="L25">
         <f t="shared" si="2"/>
@@ -43235,7 +43235,7 @@
       </c>
       <c r="K26" s="25">
         <f ca="1">VLOOKUP(I26,clientes!$A:$P,12,FALSE)</f>
-        <v>1566</v>
+        <v>1574</v>
       </c>
       <c r="L26">
         <f t="shared" si="2"/>
@@ -43291,7 +43291,7 @@
       </c>
       <c r="K27" s="25">
         <f ca="1">VLOOKUP(I27,clientes!$A:$P,12,FALSE)</f>
-        <v>783</v>
+        <v>791</v>
       </c>
       <c r="L27">
         <f t="shared" si="2"/>
@@ -43347,7 +43347,7 @@
       </c>
       <c r="K28" s="25">
         <f ca="1">VLOOKUP(I28,clientes!$A:$P,12,FALSE)</f>
-        <v>789</v>
+        <v>797</v>
       </c>
       <c r="L28">
         <f t="shared" si="2"/>
@@ -43403,7 +43403,7 @@
       </c>
       <c r="K29" s="25">
         <f ca="1">VLOOKUP(I29,clientes!$A:$P,12,FALSE)</f>
-        <v>868</v>
+        <v>876</v>
       </c>
       <c r="L29">
         <f t="shared" si="2"/>
@@ -43450,7 +43450,7 @@
       </c>
       <c r="K30" s="25">
         <f ca="1">VLOOKUP(I30,clientes!$A:$P,12,FALSE)</f>
-        <v>867</v>
+        <v>875</v>
       </c>
       <c r="L30">
         <f t="shared" si="2"/>
@@ -43468,10 +43468,10 @@
         <f t="shared" ca="1" si="5"/>
         <v>3</v>
       </c>
-      <c r="Q30" s="33" t="s">
+      <c r="Q30" s="34" t="s">
         <v>295</v>
       </c>
-      <c r="R30" s="33"/>
+      <c r="R30" s="34"/>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31">
@@ -43501,7 +43501,7 @@
       </c>
       <c r="K31" s="25">
         <f ca="1">VLOOKUP(I31,clientes!$A:$P,12,FALSE)</f>
-        <v>1021</v>
+        <v>1029</v>
       </c>
       <c r="L31">
         <f t="shared" si="2"/>
@@ -43557,7 +43557,7 @@
       </c>
       <c r="K32" s="25">
         <f ca="1">VLOOKUP(I32,clientes!$A:$P,12,FALSE)</f>
-        <v>1148</v>
+        <v>1156</v>
       </c>
       <c r="L32">
         <f t="shared" si="2"/>
@@ -43613,7 +43613,7 @@
       </c>
       <c r="K33" s="25">
         <f ca="1">VLOOKUP(I33,clientes!$A:$P,12,FALSE)</f>
-        <v>1598</v>
+        <v>1606</v>
       </c>
       <c r="L33">
         <f t="shared" si="2"/>
@@ -43669,7 +43669,7 @@
       </c>
       <c r="K34" s="25">
         <f ca="1">VLOOKUP(I34,clientes!$A:$P,12,FALSE)</f>
-        <v>781</v>
+        <v>789</v>
       </c>
       <c r="L34">
         <f t="shared" si="2"/>
@@ -43725,7 +43725,7 @@
       </c>
       <c r="K35" s="25">
         <f ca="1">VLOOKUP(I35,clientes!$A:$P,12,FALSE)</f>
-        <v>898</v>
+        <v>906</v>
       </c>
       <c r="L35">
         <f t="shared" si="2"/>
@@ -43741,7 +43741,7 @@
       </c>
       <c r="O35">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q35" s="11">
         <v>3</v>
@@ -43781,7 +43781,7 @@
       </c>
       <c r="K36" s="25">
         <f ca="1">VLOOKUP(I36,clientes!$A:$P,12,FALSE)</f>
-        <v>897</v>
+        <v>905</v>
       </c>
       <c r="L36">
         <f t="shared" si="2"/>
@@ -43797,7 +43797,7 @@
       </c>
       <c r="O36">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q36" s="11">
         <v>4</v>
@@ -43837,7 +43837,7 @@
       </c>
       <c r="K37" s="25">
         <f ca="1">VLOOKUP(I37,clientes!$A:$P,12,FALSE)</f>
-        <v>1085</v>
+        <v>1093</v>
       </c>
       <c r="L37">
         <f t="shared" si="2"/>
@@ -43893,7 +43893,7 @@
       </c>
       <c r="K38" s="25">
         <f ca="1">VLOOKUP(I38,clientes!$A:$P,12,FALSE)</f>
-        <v>1192</v>
+        <v>1200</v>
       </c>
       <c r="L38">
         <f t="shared" si="2"/>
@@ -43909,7 +43909,7 @@
       </c>
       <c r="O38">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.25">
@@ -43940,7 +43940,7 @@
       </c>
       <c r="K39" s="25">
         <f ca="1">VLOOKUP(I39,clientes!$A:$P,12,FALSE)</f>
-        <v>942</v>
+        <v>950</v>
       </c>
       <c r="L39">
         <f t="shared" si="2"/>
@@ -43958,10 +43958,10 @@
         <f t="shared" ca="1" si="5"/>
         <v>2</v>
       </c>
-      <c r="Q39" s="33" t="s">
+      <c r="Q39" s="34" t="s">
         <v>295</v>
       </c>
-      <c r="R39" s="33"/>
+      <c r="R39" s="34"/>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40">
@@ -43991,7 +43991,7 @@
       </c>
       <c r="K40" s="25">
         <f ca="1">VLOOKUP(I40,clientes!$A:$P,12,FALSE)</f>
-        <v>1159</v>
+        <v>1167</v>
       </c>
       <c r="L40">
         <f t="shared" si="2"/>
@@ -44047,7 +44047,7 @@
       </c>
       <c r="K41" s="25">
         <f ca="1">VLOOKUP(I41,clientes!$A:$P,12,FALSE)</f>
-        <v>1062</v>
+        <v>1070</v>
       </c>
       <c r="L41">
         <f t="shared" si="2"/>
@@ -44103,7 +44103,7 @@
       </c>
       <c r="K42" s="25">
         <f ca="1">VLOOKUP(I42,clientes!$A:$P,12,FALSE)</f>
-        <v>1186</v>
+        <v>1194</v>
       </c>
       <c r="L42">
         <f t="shared" si="2"/>
@@ -44159,7 +44159,7 @@
       </c>
       <c r="K43" s="25">
         <f ca="1">VLOOKUP(I43,clientes!$A:$P,12,FALSE)</f>
-        <v>1145</v>
+        <v>1153</v>
       </c>
       <c r="L43">
         <f t="shared" si="2"/>
@@ -44215,7 +44215,7 @@
       </c>
       <c r="K44" s="25">
         <f ca="1">VLOOKUP(I44,clientes!$A:$P,12,FALSE)</f>
-        <v>1076</v>
+        <v>1084</v>
       </c>
       <c r="L44">
         <f t="shared" si="2"/>
@@ -44271,7 +44271,7 @@
       </c>
       <c r="K45" s="25">
         <f ca="1">VLOOKUP(I45,clientes!$A:$P,12,FALSE)</f>
-        <v>1583</v>
+        <v>1591</v>
       </c>
       <c r="L45">
         <f t="shared" si="2"/>
@@ -44327,7 +44327,7 @@
       </c>
       <c r="K46" s="25">
         <f ca="1">VLOOKUP(I46,clientes!$A:$P,12,FALSE)</f>
-        <v>1686</v>
+        <v>1694</v>
       </c>
       <c r="L46">
         <f t="shared" si="2"/>
@@ -44383,7 +44383,7 @@
       </c>
       <c r="K47" s="25">
         <f ca="1">VLOOKUP(I47,clientes!$A:$P,12,FALSE)</f>
-        <v>1699</v>
+        <v>1707</v>
       </c>
       <c r="L47">
         <f t="shared" si="2"/>
@@ -44430,7 +44430,7 @@
       </c>
       <c r="K48" s="25">
         <f ca="1">VLOOKUP(I48,clientes!$A:$P,12,FALSE)</f>
-        <v>1299</v>
+        <v>1307</v>
       </c>
       <c r="L48">
         <f t="shared" si="2"/>
@@ -44477,7 +44477,7 @@
       </c>
       <c r="K49" s="25">
         <f ca="1">VLOOKUP(I49,clientes!$A:$P,12,FALSE)</f>
-        <v>1750</v>
+        <v>1758</v>
       </c>
       <c r="L49">
         <f t="shared" si="2"/>
@@ -44524,7 +44524,7 @@
       </c>
       <c r="K50" s="25">
         <f ca="1">VLOOKUP(I50,clientes!$A:$P,12,FALSE)</f>
-        <v>1613</v>
+        <v>1621</v>
       </c>
       <c r="L50">
         <f t="shared" si="2"/>
@@ -44571,7 +44571,7 @@
       </c>
       <c r="K51" s="25">
         <f ca="1">VLOOKUP(I51,clientes!$A:$P,12,FALSE)</f>
-        <v>1425</v>
+        <v>1433</v>
       </c>
       <c r="L51">
         <f t="shared" si="2"/>
@@ -44618,7 +44618,7 @@
       </c>
       <c r="K52" s="25">
         <f ca="1">VLOOKUP(I52,clientes!$A:$P,12,FALSE)</f>
-        <v>1293</v>
+        <v>1301</v>
       </c>
       <c r="L52">
         <f t="shared" si="2"/>
@@ -44665,7 +44665,7 @@
       </c>
       <c r="K53" s="25">
         <f ca="1">VLOOKUP(I53,clientes!$A:$P,12,FALSE)</f>
-        <v>1487</v>
+        <v>1495</v>
       </c>
       <c r="L53">
         <f t="shared" si="2"/>
@@ -44712,7 +44712,7 @@
       </c>
       <c r="K54" s="25">
         <f ca="1">VLOOKUP(I54,clientes!$A:$P,12,FALSE)</f>
-        <v>1451</v>
+        <v>1459</v>
       </c>
       <c r="L54">
         <f t="shared" si="2"/>
@@ -44759,7 +44759,7 @@
       </c>
       <c r="K55" s="25">
         <f ca="1">VLOOKUP(I55,clientes!$A:$P,12,FALSE)</f>
-        <v>1757</v>
+        <v>1765</v>
       </c>
       <c r="L55">
         <f t="shared" ref="L55:L86" si="7">COUNTIF(B:B,I55)</f>
@@ -44806,7 +44806,7 @@
       </c>
       <c r="K56" s="25">
         <f ca="1">VLOOKUP(I56,clientes!$A:$P,12,FALSE)</f>
-        <v>1652</v>
+        <v>1660</v>
       </c>
       <c r="L56">
         <f t="shared" si="7"/>
@@ -44853,7 +44853,7 @@
       </c>
       <c r="K57" s="25">
         <f ca="1">VLOOKUP(I57,clientes!$A:$P,12,FALSE)</f>
-        <v>799</v>
+        <v>807</v>
       </c>
       <c r="L57">
         <f t="shared" si="7"/>
@@ -44869,7 +44869,7 @@
       </c>
       <c r="O57">
         <f t="shared" ca="1" si="10"/>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.25">
@@ -44900,7 +44900,7 @@
       </c>
       <c r="K58" s="25">
         <f ca="1">VLOOKUP(I58,clientes!$A:$P,12,FALSE)</f>
-        <v>818</v>
+        <v>826</v>
       </c>
       <c r="L58">
         <f t="shared" si="7"/>
@@ -44947,7 +44947,7 @@
       </c>
       <c r="K59" s="25">
         <f ca="1">VLOOKUP(I59,clientes!$A:$P,12,FALSE)</f>
-        <v>1552</v>
+        <v>1560</v>
       </c>
       <c r="L59">
         <f t="shared" si="7"/>
@@ -44994,7 +44994,7 @@
       </c>
       <c r="K60" s="25">
         <f ca="1">VLOOKUP(I60,clientes!$A:$P,12,FALSE)</f>
-        <v>1613</v>
+        <v>1621</v>
       </c>
       <c r="L60">
         <f t="shared" si="7"/>
@@ -45041,7 +45041,7 @@
       </c>
       <c r="K61" s="25">
         <f ca="1">VLOOKUP(I61,clientes!$A:$P,12,FALSE)</f>
-        <v>1684</v>
+        <v>1692</v>
       </c>
       <c r="L61">
         <f t="shared" si="7"/>
@@ -45088,7 +45088,7 @@
       </c>
       <c r="K62" s="25">
         <f ca="1">VLOOKUP(I62,clientes!$A:$P,12,FALSE)</f>
-        <v>1525</v>
+        <v>1533</v>
       </c>
       <c r="L62">
         <f t="shared" si="7"/>
@@ -45135,7 +45135,7 @@
       </c>
       <c r="K63" s="25">
         <f ca="1">VLOOKUP(I63,clientes!$A:$P,12,FALSE)</f>
-        <v>1681</v>
+        <v>1689</v>
       </c>
       <c r="L63">
         <f t="shared" si="7"/>
@@ -45182,7 +45182,7 @@
       </c>
       <c r="K64" s="25">
         <f ca="1">VLOOKUP(I64,clientes!$A:$P,12,FALSE)</f>
-        <v>1507</v>
+        <v>1515</v>
       </c>
       <c r="L64">
         <f t="shared" si="7"/>
@@ -45229,7 +45229,7 @@
       </c>
       <c r="K65" s="25">
         <f ca="1">VLOOKUP(I65,clientes!$A:$P,12,FALSE)</f>
-        <v>1640</v>
+        <v>1648</v>
       </c>
       <c r="L65">
         <f t="shared" si="7"/>
@@ -45276,7 +45276,7 @@
       </c>
       <c r="K66" s="25">
         <f ca="1">VLOOKUP(I66,clientes!$A:$P,12,FALSE)</f>
-        <v>795</v>
+        <v>803</v>
       </c>
       <c r="L66">
         <f t="shared" si="7"/>
@@ -45292,7 +45292,7 @@
       </c>
       <c r="O66">
         <f t="shared" ca="1" si="10"/>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="67" spans="1:15" x14ac:dyDescent="0.25">
@@ -45323,7 +45323,7 @@
       </c>
       <c r="K67" s="25">
         <f ca="1">VLOOKUP(I67,clientes!$A:$P,12,FALSE)</f>
-        <v>782</v>
+        <v>790</v>
       </c>
       <c r="L67">
         <f t="shared" si="7"/>
@@ -45370,7 +45370,7 @@
       </c>
       <c r="K68" s="25">
         <f ca="1">VLOOKUP(I68,clientes!$A:$P,12,FALSE)</f>
-        <v>828</v>
+        <v>836</v>
       </c>
       <c r="L68">
         <f t="shared" si="7"/>
@@ -45417,7 +45417,7 @@
       </c>
       <c r="K69" s="25">
         <f ca="1">VLOOKUP(I69,clientes!$A:$P,12,FALSE)</f>
-        <v>1103</v>
+        <v>1111</v>
       </c>
       <c r="L69">
         <f t="shared" si="7"/>
@@ -45464,7 +45464,7 @@
       </c>
       <c r="K70" s="25">
         <f ca="1">VLOOKUP(I70,clientes!$A:$P,12,FALSE)</f>
-        <v>1092</v>
+        <v>1100</v>
       </c>
       <c r="L70">
         <f t="shared" si="7"/>
@@ -45511,7 +45511,7 @@
       </c>
       <c r="K71" s="25">
         <f ca="1">VLOOKUP(I71,clientes!$A:$P,12,FALSE)</f>
-        <v>1119</v>
+        <v>1127</v>
       </c>
       <c r="L71">
         <f t="shared" si="7"/>
@@ -45558,7 +45558,7 @@
       </c>
       <c r="K72" s="25">
         <f ca="1">VLOOKUP(I72,clientes!$A:$P,12,FALSE)</f>
-        <v>1106</v>
+        <v>1114</v>
       </c>
       <c r="L72">
         <f t="shared" si="7"/>
@@ -45605,7 +45605,7 @@
       </c>
       <c r="K73" s="25">
         <f ca="1">VLOOKUP(I73,clientes!$A:$P,12,FALSE)</f>
-        <v>1163</v>
+        <v>1171</v>
       </c>
       <c r="L73">
         <f t="shared" si="7"/>
@@ -45652,7 +45652,7 @@
       </c>
       <c r="K74" s="25">
         <f ca="1">VLOOKUP(I74,clientes!$A:$P,12,FALSE)</f>
-        <v>976</v>
+        <v>984</v>
       </c>
       <c r="L74">
         <f t="shared" si="7"/>
@@ -45699,7 +45699,7 @@
       </c>
       <c r="K75" s="25">
         <f ca="1">VLOOKUP(I75,clientes!$A:$P,12,FALSE)</f>
-        <v>1270</v>
+        <v>1278</v>
       </c>
       <c r="L75">
         <f t="shared" si="7"/>
@@ -45746,7 +45746,7 @@
       </c>
       <c r="K76" s="25">
         <f ca="1">VLOOKUP(I76,clientes!$A:$P,12,FALSE)</f>
-        <v>1493</v>
+        <v>1501</v>
       </c>
       <c r="L76">
         <f t="shared" si="7"/>
@@ -45793,7 +45793,7 @@
       </c>
       <c r="K77" s="25">
         <f ca="1">VLOOKUP(I77,clientes!$A:$P,12,FALSE)</f>
-        <v>1546</v>
+        <v>1554</v>
       </c>
       <c r="L77">
         <f t="shared" si="7"/>
@@ -45840,7 +45840,7 @@
       </c>
       <c r="K78" s="25">
         <f ca="1">VLOOKUP(I78,clientes!$A:$P,12,FALSE)</f>
-        <v>1728</v>
+        <v>1736</v>
       </c>
       <c r="L78">
         <f t="shared" si="7"/>
@@ -45887,7 +45887,7 @@
       </c>
       <c r="K79" s="25">
         <f ca="1">VLOOKUP(I79,clientes!$A:$P,12,FALSE)</f>
-        <v>1484</v>
+        <v>1492</v>
       </c>
       <c r="L79">
         <f t="shared" si="7"/>
@@ -45934,7 +45934,7 @@
       </c>
       <c r="K80" s="25">
         <f ca="1">VLOOKUP(I80,clientes!$A:$P,12,FALSE)</f>
-        <v>1381</v>
+        <v>1389</v>
       </c>
       <c r="L80">
         <f t="shared" si="7"/>
@@ -45981,7 +45981,7 @@
       </c>
       <c r="K81" s="25">
         <f ca="1">VLOOKUP(I81,clientes!$A:$P,12,FALSE)</f>
-        <v>1339</v>
+        <v>1347</v>
       </c>
       <c r="L81">
         <f t="shared" si="7"/>
@@ -46028,7 +46028,7 @@
       </c>
       <c r="K82" s="25">
         <f ca="1">VLOOKUP(I82,clientes!$A:$P,12,FALSE)</f>
-        <v>1503</v>
+        <v>1511</v>
       </c>
       <c r="L82">
         <f t="shared" si="7"/>
@@ -46075,7 +46075,7 @@
       </c>
       <c r="K83" s="25">
         <f ca="1">VLOOKUP(I83,clientes!$A:$P,12,FALSE)</f>
-        <v>1251</v>
+        <v>1259</v>
       </c>
       <c r="L83">
         <f t="shared" si="7"/>
@@ -46122,7 +46122,7 @@
       </c>
       <c r="K84" s="25">
         <f ca="1">VLOOKUP(I84,clientes!$A:$P,12,FALSE)</f>
-        <v>1743</v>
+        <v>1751</v>
       </c>
       <c r="L84">
         <f t="shared" si="7"/>
@@ -46169,7 +46169,7 @@
       </c>
       <c r="K85" s="25">
         <f ca="1">VLOOKUP(I85,clientes!$A:$P,12,FALSE)</f>
-        <v>1521</v>
+        <v>1529</v>
       </c>
       <c r="L85">
         <f t="shared" si="7"/>
@@ -46216,7 +46216,7 @@
       </c>
       <c r="K86" s="25">
         <f ca="1">VLOOKUP(I86,clientes!$A:$P,12,FALSE)</f>
-        <v>931</v>
+        <v>939</v>
       </c>
       <c r="L86">
         <f t="shared" si="7"/>
@@ -46263,7 +46263,7 @@
       </c>
       <c r="K87" s="25">
         <f ca="1">VLOOKUP(I87,clientes!$A:$P,12,FALSE)</f>
-        <v>1133</v>
+        <v>1141</v>
       </c>
       <c r="L87">
         <f t="shared" ref="L87:L118" si="12">COUNTIF(B:B,I87)</f>
@@ -46310,7 +46310,7 @@
       </c>
       <c r="K88" s="25">
         <f ca="1">VLOOKUP(I88,clientes!$A:$P,12,FALSE)</f>
-        <v>1381</v>
+        <v>1389</v>
       </c>
       <c r="L88">
         <f t="shared" si="12"/>
@@ -46357,7 +46357,7 @@
       </c>
       <c r="K89" s="25">
         <f ca="1">VLOOKUP(I89,clientes!$A:$P,12,FALSE)</f>
-        <v>1646</v>
+        <v>1654</v>
       </c>
       <c r="L89">
         <f t="shared" si="12"/>
@@ -46404,7 +46404,7 @@
       </c>
       <c r="K90" s="25">
         <f ca="1">VLOOKUP(I90,clientes!$A:$P,12,FALSE)</f>
-        <v>1665</v>
+        <v>1673</v>
       </c>
       <c r="L90">
         <f t="shared" si="12"/>
@@ -46451,7 +46451,7 @@
       </c>
       <c r="K91" s="25">
         <f ca="1">VLOOKUP(I91,clientes!$A:$P,12,FALSE)</f>
-        <v>1288</v>
+        <v>1296</v>
       </c>
       <c r="L91">
         <f t="shared" si="12"/>
@@ -46498,7 +46498,7 @@
       </c>
       <c r="K92" s="25">
         <f ca="1">VLOOKUP(I92,clientes!$A:$P,12,FALSE)</f>
-        <v>805</v>
+        <v>813</v>
       </c>
       <c r="L92">
         <f t="shared" si="12"/>
@@ -46545,7 +46545,7 @@
       </c>
       <c r="K93" s="25">
         <f ca="1">VLOOKUP(I93,clientes!$A:$P,12,FALSE)</f>
-        <v>828</v>
+        <v>836</v>
       </c>
       <c r="L93">
         <f t="shared" si="12"/>
@@ -46592,7 +46592,7 @@
       </c>
       <c r="K94" s="25">
         <f ca="1">VLOOKUP(I94,clientes!$A:$P,12,FALSE)</f>
-        <v>1163</v>
+        <v>1171</v>
       </c>
       <c r="L94">
         <f t="shared" si="12"/>
@@ -46639,7 +46639,7 @@
       </c>
       <c r="K95" s="25">
         <f ca="1">VLOOKUP(I95,clientes!$A:$P,12,FALSE)</f>
-        <v>1002</v>
+        <v>1010</v>
       </c>
       <c r="L95">
         <f t="shared" si="12"/>
@@ -46686,7 +46686,7 @@
       </c>
       <c r="K96" s="25">
         <f ca="1">VLOOKUP(I96,clientes!$A:$P,12,FALSE)</f>
-        <v>1155</v>
+        <v>1163</v>
       </c>
       <c r="L96">
         <f t="shared" si="12"/>
@@ -46733,7 +46733,7 @@
       </c>
       <c r="K97" s="25">
         <f ca="1">VLOOKUP(I97,clientes!$A:$P,12,FALSE)</f>
-        <v>945</v>
+        <v>953</v>
       </c>
       <c r="L97">
         <f t="shared" si="12"/>
@@ -46780,7 +46780,7 @@
       </c>
       <c r="K98" s="25">
         <f ca="1">VLOOKUP(I98,clientes!$A:$P,12,FALSE)</f>
-        <v>910</v>
+        <v>918</v>
       </c>
       <c r="L98">
         <f t="shared" si="12"/>
@@ -46827,7 +46827,7 @@
       </c>
       <c r="K99" s="25">
         <f ca="1">VLOOKUP(I99,clientes!$A:$P,12,FALSE)</f>
-        <v>954</v>
+        <v>962</v>
       </c>
       <c r="L99">
         <f t="shared" si="12"/>
@@ -46874,7 +46874,7 @@
       </c>
       <c r="K100" s="25">
         <f ca="1">VLOOKUP(I100,clientes!$A:$P,12,FALSE)</f>
-        <v>1223</v>
+        <v>1231</v>
       </c>
       <c r="L100">
         <f t="shared" si="12"/>
@@ -46921,7 +46921,7 @@
       </c>
       <c r="K101" s="25">
         <f ca="1">VLOOKUP(I101,clientes!$A:$P,12,FALSE)</f>
-        <v>1659</v>
+        <v>1667</v>
       </c>
       <c r="L101">
         <f t="shared" si="12"/>
@@ -46968,7 +46968,7 @@
       </c>
       <c r="K102" s="25">
         <f ca="1">VLOOKUP(I102,clientes!$A:$P,12,FALSE)</f>
-        <v>1461</v>
+        <v>1469</v>
       </c>
       <c r="L102">
         <f t="shared" si="12"/>
@@ -47015,7 +47015,7 @@
       </c>
       <c r="K103" s="25">
         <f ca="1">VLOOKUP(I103,clientes!$A:$P,12,FALSE)</f>
-        <v>1420</v>
+        <v>1428</v>
       </c>
       <c r="L103">
         <f t="shared" si="12"/>
@@ -47062,7 +47062,7 @@
       </c>
       <c r="K104" s="25">
         <f ca="1">VLOOKUP(I104,clientes!$A:$P,12,FALSE)</f>
-        <v>1308</v>
+        <v>1316</v>
       </c>
       <c r="L104">
         <f t="shared" si="12"/>
@@ -47109,7 +47109,7 @@
       </c>
       <c r="K105" s="25">
         <f ca="1">VLOOKUP(I105,clientes!$A:$P,12,FALSE)</f>
-        <v>1331</v>
+        <v>1339</v>
       </c>
       <c r="L105">
         <f t="shared" si="12"/>
@@ -47156,7 +47156,7 @@
       </c>
       <c r="K106" s="25">
         <f ca="1">VLOOKUP(I106,clientes!$A:$P,12,FALSE)</f>
-        <v>1323</v>
+        <v>1331</v>
       </c>
       <c r="L106">
         <f t="shared" si="12"/>
@@ -47203,7 +47203,7 @@
       </c>
       <c r="K107" s="25">
         <f ca="1">VLOOKUP(I107,clientes!$A:$P,12,FALSE)</f>
-        <v>1718</v>
+        <v>1726</v>
       </c>
       <c r="L107">
         <f t="shared" si="12"/>
@@ -47250,7 +47250,7 @@
       </c>
       <c r="K108" s="25">
         <f ca="1">VLOOKUP(I108,clientes!$A:$P,12,FALSE)</f>
-        <v>1411</v>
+        <v>1419</v>
       </c>
       <c r="L108">
         <f t="shared" si="12"/>
@@ -47297,7 +47297,7 @@
       </c>
       <c r="K109" s="25">
         <f ca="1">VLOOKUP(I109,clientes!$A:$P,12,FALSE)</f>
-        <v>1363</v>
+        <v>1371</v>
       </c>
       <c r="L109">
         <f t="shared" si="12"/>
@@ -47344,7 +47344,7 @@
       </c>
       <c r="K110" s="25">
         <f ca="1">VLOOKUP(I110,clientes!$A:$P,12,FALSE)</f>
-        <v>1574</v>
+        <v>1582</v>
       </c>
       <c r="L110">
         <f t="shared" si="12"/>
@@ -47391,7 +47391,7 @@
       </c>
       <c r="K111" s="25">
         <f ca="1">VLOOKUP(I111,clientes!$A:$P,12,FALSE)</f>
-        <v>1304</v>
+        <v>1312</v>
       </c>
       <c r="L111">
         <f t="shared" si="12"/>
@@ -47438,7 +47438,7 @@
       </c>
       <c r="K112" s="25">
         <f ca="1">VLOOKUP(I112,clientes!$A:$P,12,FALSE)</f>
-        <v>1263</v>
+        <v>1271</v>
       </c>
       <c r="L112">
         <f t="shared" si="12"/>
@@ -47485,7 +47485,7 @@
       </c>
       <c r="K113" s="25">
         <f ca="1">VLOOKUP(I113,clientes!$A:$P,12,FALSE)</f>
-        <v>1540</v>
+        <v>1548</v>
       </c>
       <c r="L113">
         <f t="shared" si="12"/>
@@ -47532,7 +47532,7 @@
       </c>
       <c r="K114" s="25">
         <f ca="1">VLOOKUP(I114,clientes!$A:$P,12,FALSE)</f>
-        <v>1091</v>
+        <v>1099</v>
       </c>
       <c r="L114">
         <f t="shared" si="12"/>
@@ -47579,7 +47579,7 @@
       </c>
       <c r="K115" s="25">
         <f ca="1">VLOOKUP(I115,clientes!$A:$P,12,FALSE)</f>
-        <v>1132</v>
+        <v>1140</v>
       </c>
       <c r="L115">
         <f t="shared" si="12"/>
@@ -47626,7 +47626,7 @@
       </c>
       <c r="K116" s="25">
         <f ca="1">VLOOKUP(I116,clientes!$A:$P,12,FALSE)</f>
-        <v>1018</v>
+        <v>1026</v>
       </c>
       <c r="L116">
         <f t="shared" si="12"/>
@@ -47673,7 +47673,7 @@
       </c>
       <c r="K117" s="25">
         <f ca="1">VLOOKUP(I117,clientes!$A:$P,12,FALSE)</f>
-        <v>1518</v>
+        <v>1526</v>
       </c>
       <c r="L117">
         <f t="shared" si="12"/>
@@ -47720,7 +47720,7 @@
       </c>
       <c r="K118" s="25">
         <f ca="1">VLOOKUP(I118,clientes!$A:$P,12,FALSE)</f>
-        <v>786</v>
+        <v>794</v>
       </c>
       <c r="L118">
         <f t="shared" si="12"/>
@@ -47767,7 +47767,7 @@
       </c>
       <c r="K119" s="25">
         <f ca="1">VLOOKUP(I119,clientes!$A:$P,12,FALSE)</f>
-        <v>869</v>
+        <v>877</v>
       </c>
       <c r="L119">
         <f t="shared" ref="L119:L154" si="17">COUNTIF(B:B,I119)</f>
@@ -47814,7 +47814,7 @@
       </c>
       <c r="K120" s="25">
         <f ca="1">VLOOKUP(I120,clientes!$A:$P,12,FALSE)</f>
-        <v>1004</v>
+        <v>1012</v>
       </c>
       <c r="L120">
         <f t="shared" si="17"/>
@@ -47861,7 +47861,7 @@
       </c>
       <c r="K121" s="25">
         <f ca="1">VLOOKUP(I121,clientes!$A:$P,12,FALSE)</f>
-        <v>1111</v>
+        <v>1119</v>
       </c>
       <c r="L121">
         <f t="shared" si="17"/>
@@ -47908,7 +47908,7 @@
       </c>
       <c r="K122" s="25">
         <f ca="1">VLOOKUP(I122,clientes!$A:$P,12,FALSE)</f>
-        <v>1200</v>
+        <v>1208</v>
       </c>
       <c r="L122">
         <f t="shared" si="17"/>
@@ -47955,7 +47955,7 @@
       </c>
       <c r="K123" s="25">
         <f ca="1">VLOOKUP(I123,clientes!$A:$P,12,FALSE)</f>
-        <v>1177</v>
+        <v>1185</v>
       </c>
       <c r="L123">
         <f t="shared" si="17"/>
@@ -48002,7 +48002,7 @@
       </c>
       <c r="K124" s="25">
         <f ca="1">VLOOKUP(I124,clientes!$A:$P,12,FALSE)</f>
-        <v>1056</v>
+        <v>1064</v>
       </c>
       <c r="L124">
         <f t="shared" si="17"/>
@@ -48049,7 +48049,7 @@
       </c>
       <c r="K125" s="25">
         <f ca="1">VLOOKUP(I125,clientes!$A:$P,12,FALSE)</f>
-        <v>1727</v>
+        <v>1735</v>
       </c>
       <c r="L125">
         <f t="shared" si="17"/>
@@ -48096,7 +48096,7 @@
       </c>
       <c r="K126" s="25">
         <f ca="1">VLOOKUP(I126,clientes!$A:$P,12,FALSE)</f>
-        <v>1414</v>
+        <v>1422</v>
       </c>
       <c r="L126">
         <f t="shared" si="17"/>
@@ -48143,7 +48143,7 @@
       </c>
       <c r="K127" s="25">
         <f ca="1">VLOOKUP(I127,clientes!$A:$P,12,FALSE)</f>
-        <v>1399</v>
+        <v>1407</v>
       </c>
       <c r="L127">
         <f t="shared" si="17"/>
@@ -48190,7 +48190,7 @@
       </c>
       <c r="K128" s="25">
         <f ca="1">VLOOKUP(I128,clientes!$A:$P,12,FALSE)</f>
-        <v>1240</v>
+        <v>1248</v>
       </c>
       <c r="L128">
         <f t="shared" si="17"/>
@@ -48237,7 +48237,7 @@
       </c>
       <c r="K129" s="25">
         <f ca="1">VLOOKUP(I129,clientes!$A:$P,12,FALSE)</f>
-        <v>1602</v>
+        <v>1610</v>
       </c>
       <c r="L129">
         <f t="shared" si="17"/>
@@ -48284,7 +48284,7 @@
       </c>
       <c r="K130" s="25">
         <f ca="1">VLOOKUP(I130,clientes!$A:$P,12,FALSE)</f>
-        <v>1217</v>
+        <v>1225</v>
       </c>
       <c r="L130">
         <f t="shared" si="17"/>
@@ -48331,7 +48331,7 @@
       </c>
       <c r="K131" s="25">
         <f ca="1">VLOOKUP(I131,clientes!$A:$P,12,FALSE)</f>
-        <v>1294</v>
+        <v>1302</v>
       </c>
       <c r="L131">
         <f t="shared" si="17"/>
@@ -48378,7 +48378,7 @@
       </c>
       <c r="K132" s="25">
         <f ca="1">VLOOKUP(I132,clientes!$A:$P,12,FALSE)</f>
-        <v>1293</v>
+        <v>1301</v>
       </c>
       <c r="L132">
         <f t="shared" si="17"/>
@@ -48425,7 +48425,7 @@
       </c>
       <c r="K133" s="25">
         <f ca="1">VLOOKUP(I133,clientes!$A:$P,12,FALSE)</f>
-        <v>1699</v>
+        <v>1707</v>
       </c>
       <c r="L133">
         <f t="shared" si="17"/>
@@ -48472,7 +48472,7 @@
       </c>
       <c r="K134" s="25">
         <f ca="1">VLOOKUP(I134,clientes!$A:$P,12,FALSE)</f>
-        <v>1439</v>
+        <v>1447</v>
       </c>
       <c r="L134">
         <f t="shared" si="17"/>
@@ -48519,7 +48519,7 @@
       </c>
       <c r="K135" s="25">
         <f ca="1">VLOOKUP(I135,clientes!$A:$P,12,FALSE)</f>
-        <v>1520</v>
+        <v>1528</v>
       </c>
       <c r="L135">
         <f t="shared" si="17"/>
@@ -48566,7 +48566,7 @@
       </c>
       <c r="K136" s="25">
         <f ca="1">VLOOKUP(I136,clientes!$A:$P,12,FALSE)</f>
-        <v>1495</v>
+        <v>1503</v>
       </c>
       <c r="L136">
         <f t="shared" si="17"/>
@@ -48613,7 +48613,7 @@
       </c>
       <c r="K137" s="25">
         <f ca="1">VLOOKUP(I137,clientes!$A:$P,12,FALSE)</f>
-        <v>1392</v>
+        <v>1400</v>
       </c>
       <c r="L137">
         <f t="shared" si="17"/>
@@ -48660,7 +48660,7 @@
       </c>
       <c r="K138" s="25">
         <f ca="1">VLOOKUP(I138,clientes!$A:$P,12,FALSE)</f>
-        <v>1759</v>
+        <v>1767</v>
       </c>
       <c r="L138">
         <f t="shared" si="17"/>
@@ -48707,7 +48707,7 @@
       </c>
       <c r="K139" s="25">
         <f ca="1">VLOOKUP(I139,clientes!$A:$P,12,FALSE)</f>
-        <v>868</v>
+        <v>876</v>
       </c>
       <c r="L139">
         <f t="shared" si="17"/>
@@ -48754,7 +48754,7 @@
       </c>
       <c r="K140" s="25">
         <f ca="1">VLOOKUP(I140,clientes!$A:$P,12,FALSE)</f>
-        <v>841</v>
+        <v>849</v>
       </c>
       <c r="L140">
         <f t="shared" si="17"/>
@@ -48801,7 +48801,7 @@
       </c>
       <c r="K141" s="25">
         <f ca="1">VLOOKUP(I141,clientes!$A:$P,12,FALSE)</f>
-        <v>857</v>
+        <v>865</v>
       </c>
       <c r="L141">
         <f t="shared" si="17"/>
@@ -48848,7 +48848,7 @@
       </c>
       <c r="K142" s="25">
         <f ca="1">VLOOKUP(I142,clientes!$A:$P,12,FALSE)</f>
-        <v>900</v>
+        <v>908</v>
       </c>
       <c r="L142">
         <f t="shared" si="17"/>
@@ -48895,7 +48895,7 @@
       </c>
       <c r="K143" s="25">
         <f ca="1">VLOOKUP(I143,clientes!$A:$P,12,FALSE)</f>
-        <v>1180</v>
+        <v>1188</v>
       </c>
       <c r="L143">
         <f t="shared" si="17"/>
@@ -48942,7 +48942,7 @@
       </c>
       <c r="K144" s="25">
         <f ca="1">VLOOKUP(I144,clientes!$A:$P,12,FALSE)</f>
-        <v>921</v>
+        <v>929</v>
       </c>
       <c r="L144">
         <f t="shared" si="17"/>
@@ -48989,7 +48989,7 @@
       </c>
       <c r="K145" s="25">
         <f ca="1">VLOOKUP(I145,clientes!$A:$P,12,FALSE)</f>
-        <v>918</v>
+        <v>926</v>
       </c>
       <c r="L145">
         <f t="shared" si="17"/>
@@ -49036,7 +49036,7 @@
       </c>
       <c r="K146" s="25">
         <f ca="1">VLOOKUP(I146,clientes!$A:$P,12,FALSE)</f>
-        <v>927</v>
+        <v>935</v>
       </c>
       <c r="L146">
         <f t="shared" si="17"/>
@@ -49083,7 +49083,7 @@
       </c>
       <c r="K147" s="25">
         <f ca="1">VLOOKUP(I147,clientes!$A:$P,12,FALSE)</f>
-        <v>1139</v>
+        <v>1147</v>
       </c>
       <c r="L147">
         <f t="shared" si="17"/>
@@ -49130,7 +49130,7 @@
       </c>
       <c r="K148" s="25">
         <f ca="1">VLOOKUP(I148,clientes!$A:$P,12,FALSE)</f>
-        <v>1069</v>
+        <v>1077</v>
       </c>
       <c r="L148">
         <f t="shared" si="17"/>
@@ -49177,7 +49177,7 @@
       </c>
       <c r="K149" s="25">
         <f ca="1">VLOOKUP(I149,clientes!$A:$P,12,FALSE)</f>
-        <v>1406</v>
+        <v>1414</v>
       </c>
       <c r="L149">
         <f t="shared" si="17"/>
@@ -49224,7 +49224,7 @@
       </c>
       <c r="K150" s="25">
         <f ca="1">VLOOKUP(I150,clientes!$A:$P,12,FALSE)</f>
-        <v>1631</v>
+        <v>1639</v>
       </c>
       <c r="L150">
         <f t="shared" si="17"/>
@@ -49271,7 +49271,7 @@
       </c>
       <c r="K151" s="25">
         <f ca="1">VLOOKUP(I151,clientes!$A:$P,12,FALSE)</f>
-        <v>1511</v>
+        <v>1519</v>
       </c>
       <c r="L151">
         <f t="shared" si="17"/>
@@ -49318,7 +49318,7 @@
       </c>
       <c r="K152" s="25">
         <f ca="1">VLOOKUP(I152,clientes!$A:$P,12,FALSE)</f>
-        <v>1285</v>
+        <v>1293</v>
       </c>
       <c r="L152">
         <f t="shared" si="17"/>
@@ -49365,7 +49365,7 @@
       </c>
       <c r="K153" s="25">
         <f ca="1">VLOOKUP(I153,clientes!$A:$P,12,FALSE)</f>
-        <v>1224</v>
+        <v>1232</v>
       </c>
       <c r="L153">
         <f t="shared" si="17"/>
@@ -49412,7 +49412,7 @@
       </c>
       <c r="K154" s="25">
         <f ca="1">VLOOKUP(I154,clientes!$A:$P,12,FALSE)</f>
-        <v>1740</v>
+        <v>1748</v>
       </c>
       <c r="L154">
         <f t="shared" si="17"/>
@@ -54616,27 +54616,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="str">
+      <c r="A1" s="34" t="str">
         <f>transacoes!I21</f>
         <v>Clientes de alto valor</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
       <c r="E1" s="22"/>
       <c r="F1" s="22"/>
-      <c r="H1" s="33" t="s">
+      <c r="H1" s="34" t="s">
         <v>295</v>
       </c>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="M1" s="33" t="str">
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
+      <c r="M1" s="34" t="str">
         <f>transacoes!Q39</f>
         <v>Classificação</v>
       </c>
-      <c r="N1" s="33"/>
-      <c r="O1" s="33"/>
+      <c r="N1" s="34"/>
+      <c r="O1" s="34"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
@@ -55052,12 +55052,12 @@
       <c r="K10">
         <v>4</v>
       </c>
-      <c r="M10" s="33" t="str">
+      <c r="M10" s="34" t="str">
         <f>transacoes!Q30</f>
         <v>Classificação</v>
       </c>
-      <c r="N10" s="33"/>
-      <c r="O10" s="33"/>
+      <c r="N10" s="34"/>
+      <c r="O10" s="34"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="21">
@@ -55122,15 +55122,15 @@
       </c>
       <c r="D12">
         <f ca="1">transacoes!O35</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="F12" t="str" cm="1">
         <f t="array" aca="1" ref="F12" ca="1">_xlfn.IFS(AND(D12&gt;=4,D12&lt;=5,E12&gt;=4,E12&lt;=5),"Campeões",AND(D12&gt;=2,D12&lt;=5,E12&gt;=3,E12&lt;=5),"Clientes fieis",AND(D12&gt;=3,D12&lt;=5,E12&gt;=1,E12&lt;=3),"Lealdade potencial",AND(D12&gt;=4,D12&lt;=5,E12&gt;=0,E12&lt;=1),"Clientes recentes",AND(D12&gt;=3,D12&lt;=4,E12&gt;=0,E12&lt;=1),"Promissor",AND(D12&gt;=2,D12&lt;=3,E12&gt;=2,E12&lt;=3),"Clientes que precisam de atenção",AND(D12&gt;=2,D12&lt;=3,E12&gt;=0,E12&lt;=2),"Prestes a hibernar",AND(D12&gt;=0,D12&lt;=2,E12&gt;=2,E12&lt;=5),"Em risco",AND(D12&gt;=0,D12&lt;=1,E12&gt;=4,E12&lt;=5),"Não posso perdê-los",AND(D12&gt;=1,D12&lt;=2,E12&gt;=1,E12&lt;=2),"Hibernando",AND(D12&gt;=0,D12&lt;=2,E12&gt;=0,E12&lt;=2),"Perdido")</f>
-        <v>Clientes fieis</v>
+        <v>Clientes que precisam de atenção</v>
       </c>
       <c r="H12" t="s">
         <v>328</v>
@@ -55171,15 +55171,15 @@
       </c>
       <c r="D13">
         <f ca="1">transacoes!O36</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="F13" t="str" cm="1">
         <f t="array" aca="1" ref="F13" ca="1">_xlfn.IFS(AND(D13&gt;=4,D13&lt;=5,E13&gt;=4,E13&lt;=5),"Campeões",AND(D13&gt;=2,D13&lt;=5,E13&gt;=3,E13&lt;=5),"Clientes fieis",AND(D13&gt;=3,D13&lt;=5,E13&gt;=1,E13&lt;=3),"Lealdade potencial",AND(D13&gt;=4,D13&lt;=5,E13&gt;=0,E13&lt;=1),"Clientes recentes",AND(D13&gt;=3,D13&lt;=4,E13&gt;=0,E13&lt;=1),"Promissor",AND(D13&gt;=2,D13&lt;=3,E13&gt;=2,E13&lt;=3),"Clientes que precisam de atenção",AND(D13&gt;=2,D13&lt;=3,E13&gt;=0,E13&lt;=2),"Prestes a hibernar",AND(D13&gt;=0,D13&lt;=2,E13&gt;=2,E13&lt;=5),"Em risco",AND(D13&gt;=0,D13&lt;=1,E13&gt;=4,E13&lt;=5),"Não posso perdê-los",AND(D13&gt;=1,D13&lt;=2,E13&gt;=1,E13&lt;=2),"Hibernando",AND(D13&gt;=0,D13&lt;=2,E13&gt;=0,E13&lt;=2),"Perdido")</f>
-        <v>Clientes fieis</v>
+        <v>Clientes que precisam de atenção</v>
       </c>
       <c r="H13" t="s">
         <v>330</v>
@@ -55220,11 +55220,11 @@
       </c>
       <c r="D14">
         <f ca="1">transacoes!O57</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="0"/>
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="F14" t="str" cm="1">
         <f t="array" aca="1" ref="F14" ca="1">_xlfn.IFS(AND(D14&gt;=4,D14&lt;=5,E14&gt;=4,E14&lt;=5),"Campeões",AND(D14&gt;=2,D14&lt;=5,E14&gt;=3,E14&lt;=5),"Clientes fieis",AND(D14&gt;=3,D14&lt;=5,E14&gt;=1,E14&lt;=3),"Lealdade potencial",AND(D14&gt;=4,D14&lt;=5,E14&gt;=0,E14&lt;=1),"Clientes recentes",AND(D14&gt;=3,D14&lt;=4,E14&gt;=0,E14&lt;=1),"Promissor",AND(D14&gt;=2,D14&lt;=3,E14&gt;=2,E14&lt;=3),"Clientes que precisam de atenção",AND(D14&gt;=2,D14&lt;=3,E14&gt;=0,E14&lt;=2),"Prestes a hibernar",AND(D14&gt;=0,D14&lt;=2,E14&gt;=2,E14&lt;=5),"Em risco",AND(D14&gt;=0,D14&lt;=1,E14&gt;=4,E14&lt;=5),"Não posso perdê-los",AND(D14&gt;=1,D14&lt;=2,E14&gt;=1,E14&lt;=2),"Hibernando",AND(D14&gt;=0,D14&lt;=2,E14&gt;=0,E14&lt;=2),"Perdido")</f>
@@ -55294,15 +55294,15 @@
       </c>
       <c r="D16">
         <f ca="1">transacoes!O66</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="0"/>
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="F16" t="str" cm="1">
         <f t="array" aca="1" ref="F16" ca="1">_xlfn.IFS(AND(D16&gt;=4,D16&lt;=5,E16&gt;=4,E16&lt;=5),"Campeões",AND(D16&gt;=2,D16&lt;=5,E16&gt;=3,E16&lt;=5),"Clientes fieis",AND(D16&gt;=3,D16&lt;=5,E16&gt;=1,E16&lt;=3),"Lealdade potencial",AND(D16&gt;=4,D16&lt;=5,E16&gt;=0,E16&lt;=1),"Clientes recentes",AND(D16&gt;=3,D16&lt;=4,E16&gt;=0,E16&lt;=1),"Promissor",AND(D16&gt;=2,D16&lt;=3,E16&gt;=2,E16&lt;=3),"Clientes que precisam de atenção",AND(D16&gt;=2,D16&lt;=3,E16&gt;=0,E16&lt;=2),"Prestes a hibernar",AND(D16&gt;=0,D16&lt;=2,E16&gt;=2,E16&lt;=5),"Em risco",AND(D16&gt;=0,D16&lt;=1,E16&gt;=4,E16&lt;=5),"Não posso perdê-los",AND(D16&gt;=1,D16&lt;=2,E16&gt;=1,E16&lt;=2),"Hibernando",AND(D16&gt;=0,D16&lt;=2,E16&gt;=0,E16&lt;=2),"Perdido")</f>
-        <v>Clientes fieis</v>
+        <v>Lealdade potencial</v>
       </c>
       <c r="M16" s="11">
         <f>transacoes!Q36</f>
@@ -55403,12 +55403,12 @@
         <f t="array" aca="1" ref="F19" ca="1">_xlfn.IFS(AND(D19&gt;=4,D19&lt;=5,E19&gt;=4,E19&lt;=5),"Campeões",AND(D19&gt;=2,D19&lt;=5,E19&gt;=3,E19&lt;=5),"Clientes fieis",AND(D19&gt;=3,D19&lt;=5,E19&gt;=1,E19&lt;=3),"Lealdade potencial",AND(D19&gt;=4,D19&lt;=5,E19&gt;=0,E19&lt;=1),"Clientes recentes",AND(D19&gt;=3,D19&lt;=4,E19&gt;=0,E19&lt;=1),"Promissor",AND(D19&gt;=2,D19&lt;=3,E19&gt;=2,E19&lt;=3),"Clientes que precisam de atenção",AND(D19&gt;=2,D19&lt;=3,E19&gt;=0,E19&lt;=2),"Prestes a hibernar",AND(D19&gt;=0,D19&lt;=2,E19&gt;=2,E19&lt;=5),"Em risco",AND(D19&gt;=0,D19&lt;=1,E19&gt;=4,E19&lt;=5),"Não posso perdê-los",AND(D19&gt;=1,D19&lt;=2,E19&gt;=1,E19&lt;=2),"Hibernando",AND(D19&gt;=0,D19&lt;=2,E19&gt;=0,E19&lt;=2),"Perdido")</f>
         <v>Lealdade potencial</v>
       </c>
-      <c r="M19" s="33" t="str">
+      <c r="M19" s="34" t="str">
         <f>transacoes!Q21</f>
         <v>Classificação arrecadação</v>
       </c>
-      <c r="N19" s="33"/>
-      <c r="O19" s="33"/>
+      <c r="N19" s="34"/>
+      <c r="O19" s="34"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" s="21">
@@ -55708,15 +55708,15 @@
       </c>
       <c r="D28">
         <f ca="1">transacoes!O38</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E28">
         <f t="shared" ca="1" si="0"/>
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="F28" t="str" cm="1">
         <f t="array" aca="1" ref="F28" ca="1">_xlfn.IFS(AND(D28&gt;=4,D28&lt;=5,E28&gt;=4,E28&lt;=5),"Campeões",AND(D28&gt;=2,D28&lt;=5,E28&gt;=3,E28&lt;=5),"Clientes fieis",AND(D28&gt;=3,D28&lt;=5,E28&gt;=1,E28&lt;=3),"Lealdade potencial",AND(D28&gt;=4,D28&lt;=5,E28&gt;=0,E28&lt;=1),"Clientes recentes",AND(D28&gt;=3,D28&lt;=4,E28&gt;=0,E28&lt;=1),"Promissor",AND(D28&gt;=2,D28&lt;=3,E28&gt;=2,E28&lt;=3),"Clientes que precisam de atenção",AND(D28&gt;=2,D28&lt;=3,E28&gt;=0,E28&lt;=2),"Prestes a hibernar",AND(D28&gt;=0,D28&lt;=2,E28&gt;=2,E28&lt;=5),"Em risco",AND(D28&gt;=0,D28&lt;=1,E28&gt;=4,E28&lt;=5),"Não posso perdê-los",AND(D28&gt;=1,D28&lt;=2,E28&gt;=1,E28&lt;=2),"Hibernando",AND(D28&gt;=0,D28&lt;=2,E28&gt;=0,E28&lt;=2),"Perdido")</f>
-        <v>Clientes que precisam de atenção</v>
+        <v>Em risco</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
@@ -58521,17 +58521,17 @@
       <c r="H2" s="1" t="s">
         <v>363</v>
       </c>
-      <c r="J2" s="33" t="s">
+      <c r="J2" s="34" t="s">
         <v>295</v>
       </c>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="N2" s="33" t="s">
+      <c r="K2" s="34"/>
+      <c r="L2" s="34"/>
+      <c r="N2" s="34" t="s">
         <v>295</v>
       </c>
-      <c r="O2" s="33"/>
-      <c r="P2" s="33"/>
-      <c r="Q2" s="33"/>
+      <c r="O2" s="34"/>
+      <c r="P2" s="34"/>
+      <c r="Q2" s="34"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -59919,7 +59919,7 @@
       </c>
       <c r="H45" t="str">
         <f ca="1">IFERROR(VLOOKUP(A45,'Clientes alto valor'!$A:$F,6,FALSE),"Não classificado")</f>
-        <v>Clientes fieis</v>
+        <v>Lealdade potencial</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -60586,7 +60586,7 @@
       </c>
       <c r="H68" t="str">
         <f ca="1">IFERROR(VLOOKUP(A68,'Clientes alto valor'!$A:$F,6,FALSE),"Não classificado")</f>
-        <v>Clientes que precisam de atenção</v>
+        <v>Em risco</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
@@ -63399,7 +63399,7 @@
       </c>
       <c r="H165" t="str">
         <f ca="1">IFERROR(VLOOKUP(A165,'Clientes alto valor'!$A:$F,6,FALSE),"Não classificado")</f>
-        <v>Clientes fieis</v>
+        <v>Clientes que precisam de atenção</v>
       </c>
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.25">
@@ -63921,7 +63921,7 @@
       </c>
       <c r="H183" t="str">
         <f ca="1">IFERROR(VLOOKUP(A183,'Clientes alto valor'!$A:$F,6,FALSE),"Não classificado")</f>
-        <v>Clientes fieis</v>
+        <v>Clientes que precisam de atenção</v>
       </c>
     </row>
     <row r="184" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>